<commit_message>
checked data and prepared csv with target rate changes and meeting dates
</commit_message>
<xml_diff>
--- a/TgtRateAdjustments.xlsx
+++ b/TgtRateAdjustments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\corin\Documents\Uni\M.A.HSG\MA_Arbeit\MasterThesis_NarrativesInFinance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A23037-7BDA-47D4-A528-83213DC96C4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721A5F0E-BF01-4D4A-9D58-F5AA1856EF95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{80B993A4-3DA7-4240-872A-2188DEF1878B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{80B993A4-3DA7-4240-872A-2188DEF1878B}"/>
   </bookViews>
   <sheets>
     <sheet name="TgtRateAdjustment" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>https://www.businessinsider.de/federal-reserve-chair-to-hold-press-conferences-after-every-meeting-2018-6?r=US&amp;IR=T</t>
+  </si>
+  <si>
+    <t>https://www.federalreserve.gov/monetarypolicy/openmarket_archive.htm</t>
+  </si>
+  <si>
+    <t>https://www.federalreserve.gov/monetarypolicy/openmarket.htm</t>
   </si>
 </sst>
 </file>
@@ -183,25 +189,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -223,6 +225,11 @@
     <xf numFmtId="14" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,30 +545,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E32174-ACCF-4909-B52B-590BE0998F4D}">
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="35" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="35" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -582,15 +589,18 @@
       <c r="J1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43370</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="35">
         <v>0.02</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="35">
         <v>2.2499999999999999E-2</v>
       </c>
       <c r="D2" s="2">
@@ -600,7 +610,7 @@
         <f t="shared" ref="F2:F26" si="0">B3+D2-B2</f>
         <v>0</v>
       </c>
-      <c r="G2" s="29">
+      <c r="G2" s="25">
         <f>MATCH((A2-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>1</v>
       </c>
@@ -616,15 +626,18 @@
         <f>IF(ISNA(H2),0,1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43265</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="35">
         <v>1.7500000000000002E-2</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="35">
         <v>0.02</v>
       </c>
       <c r="D3" s="2">
@@ -634,7 +647,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G3" s="29">
+      <c r="G3" s="25">
         <f>MATCH((A3-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>3</v>
       </c>
@@ -651,14 +664,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43181</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="35">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="35">
         <v>1.7500000000000002E-2</v>
       </c>
       <c r="D4" s="2">
@@ -668,7 +681,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G4" s="29">
+      <c r="G4" s="25">
         <f>MATCH((A4-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>5</v>
       </c>
@@ -685,14 +698,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43083</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="35">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="35">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D5" s="2">
@@ -702,7 +715,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="25">
         <f>MATCH((A5-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>7</v>
       </c>
@@ -719,14 +732,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>42901</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="35">
         <v>0.01</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="35">
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="D6" s="2">
@@ -736,7 +749,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="25">
         <f>MATCH((A6-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>11</v>
       </c>
@@ -753,14 +766,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>42810</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="35">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="35">
         <v>0.01</v>
       </c>
       <c r="D7" s="2">
@@ -770,7 +783,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="25">
         <f>MATCH((A7-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>13</v>
       </c>
@@ -787,14 +800,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>42719</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="35">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="35">
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="D8" s="2">
@@ -804,7 +817,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="25">
         <f>MATCH((A8-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>15</v>
       </c>
@@ -821,14 +834,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>42355</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="35">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="35">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D9" s="2">
@@ -838,7 +851,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G9" s="25">
         <f>MATCH((A9-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>23</v>
       </c>
@@ -855,23 +868,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
         <v>39798</v>
       </c>
-      <c r="B10" s="10">
-        <v>0</v>
-      </c>
-      <c r="C10" s="10">
+      <c r="B10" s="36">
+        <v>0</v>
+      </c>
+      <c r="C10" s="36">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="9">
         <v>-7.4999999999999997E-3</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="34">
         <v>-0.01</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="15">
         <f t="shared" si="0"/>
         <v>2.5000000000000005E-3</v>
       </c>
@@ -879,7 +892,7 @@
         <f>MATCH((A10-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H10" s="29">
+      <c r="H10" s="25">
         <f>MATCH(A10,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>88</v>
       </c>
@@ -892,14 +905,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
         <v>39750</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="35">
         <v>0.01</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F11" s="2">
@@ -910,7 +923,7 @@
         <f>MATCH((A11-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H11" s="29">
+      <c r="H11" s="25">
         <f>MATCH(A11,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>89</v>
       </c>
@@ -923,21 +936,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <v>39729</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="35">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G12" s="29">
+      <c r="G12" s="25">
         <f>MATCH((A12-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>90</v>
       </c>
@@ -954,14 +967,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>39568</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="35">
         <v>0.02</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>-2.5000000000000001E-3</v>
       </c>
       <c r="F13" s="2">
@@ -972,7 +985,7 @@
         <f>MATCH((A13-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H13" s="29">
+      <c r="H13" s="25">
         <f>MATCH(A13,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>96</v>
       </c>
@@ -985,14 +998,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>39525</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="35">
         <v>2.2499999999999999E-2</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <v>-7.4999999999999997E-3</v>
       </c>
       <c r="F14" s="2">
@@ -1003,7 +1016,7 @@
         <f>MATCH((A14-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H14" s="29">
+      <c r="H14" s="25">
         <f>MATCH(A14,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>97</v>
       </c>
@@ -1016,14 +1029,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>39477</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="35">
         <v>0.03</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F15" s="2">
@@ -1034,7 +1047,7 @@
         <f>MATCH((A15-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H15" s="29">
+      <c r="H15" s="25">
         <f>MATCH(A15,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>99</v>
       </c>
@@ -1047,21 +1060,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
         <v>39469</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="35">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <v>-7.4999999999999997E-3</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G16" s="29">
+      <c r="G16" s="25">
         <f>MATCH((A16-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>100</v>
       </c>
@@ -1079,13 +1092,13 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+      <c r="A17" s="5">
         <v>39427</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="35">
         <v>4.2500000000000003E-2</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <v>-2.5000000000000001E-3</v>
       </c>
       <c r="F17" s="2">
@@ -1096,7 +1109,7 @@
         <f>MATCH((A17-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H17" s="29">
+      <c r="H17" s="25">
         <f>MATCH(A17,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>102</v>
       </c>
@@ -1110,13 +1123,13 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+      <c r="A18" s="5">
         <v>39386</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="35">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="6">
         <v>-2.5000000000000001E-3</v>
       </c>
       <c r="F18" s="2">
@@ -1127,7 +1140,7 @@
         <f>MATCH((A18-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H18" s="29">
+      <c r="H18" s="25">
         <f>MATCH(A18,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>104</v>
       </c>
@@ -1141,13 +1154,13 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
+      <c r="A19" s="5">
         <v>39343</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="35">
         <v>4.7500000000000001E-2</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="6">
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F19" s="2">
@@ -1158,7 +1171,7 @@
         <f>MATCH((A19-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H19" s="29">
+      <c r="H19" s="25">
         <f>MATCH(A19,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>105</v>
       </c>
@@ -1175,10 +1188,10 @@
       <c r="A20" s="1">
         <v>38897</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="37">
         <v>5.2499999999999998E-2</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="7">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F20" s="2">
@@ -1189,7 +1202,7 @@
         <f>MATCH((A20-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H20" s="29">
+      <c r="H20" s="25">
         <f>MATCH(A20,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>117</v>
       </c>
@@ -1206,10 +1219,10 @@
       <c r="A21" s="1">
         <v>38847</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="38">
         <v>0.05</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="7">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F21" s="2">
@@ -1220,7 +1233,7 @@
         <f>MATCH((A21-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H21" s="29">
+      <c r="H21" s="25">
         <f>MATCH(A21,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>118</v>
       </c>
@@ -1237,10 +1250,10 @@
       <c r="A22" s="1">
         <v>38804</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="38">
         <v>4.7500000000000001E-2</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="7">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F22" s="2">
@@ -1251,7 +1264,7 @@
         <f>MATCH((A22-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H22" s="29">
+      <c r="H22" s="25">
         <f>MATCH(A22,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>119</v>
       </c>
@@ -1268,10 +1281,10 @@
       <c r="A23" s="1">
         <v>38748</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="38">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="7">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F23" s="2">
@@ -1282,7 +1295,7 @@
         <f>MATCH((A23-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H23" s="29">
+      <c r="H23" s="25">
         <f>MATCH(A23,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>120</v>
       </c>
@@ -1299,10 +1312,10 @@
       <c r="A24" s="1">
         <v>38699</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="38">
         <v>4.2500000000000003E-2</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D24" s="7">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F24" s="2">
@@ -1313,7 +1326,7 @@
         <f>MATCH((A24-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H24" s="29">
+      <c r="H24" s="25">
         <f>MATCH(A24,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>121</v>
       </c>
@@ -1330,10 +1343,10 @@
       <c r="A25" s="1">
         <v>38657</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25" s="38">
         <v>0.04</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="7">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F25" s="2">
@@ -1344,7 +1357,7 @@
         <f>MATCH((A25-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H25" s="29">
+      <c r="H25" s="25">
         <f>MATCH(A25,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>122</v>
       </c>
@@ -1361,10 +1374,10 @@
       <c r="A26" s="1">
         <v>38615</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B26" s="38">
         <v>3.7499999999999999E-2</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="7">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F26" s="2">
@@ -1375,7 +1388,7 @@
         <f>MATCH((A26-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H26" s="29">
+      <c r="H26" s="25">
         <f>MATCH(A26,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>123</v>
       </c>
@@ -1392,10 +1405,10 @@
       <c r="A27" s="1">
         <v>38573</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" s="38">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D27" s="7">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F27" s="2">
@@ -1406,7 +1419,7 @@
         <f>MATCH((A27-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H27" s="29">
+      <c r="H27" s="25">
         <f>MATCH(A27,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>124</v>
       </c>
@@ -1423,10 +1436,10 @@
       <c r="A28" s="1">
         <v>38533</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28" s="38">
         <v>3.2500000000000001E-2</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D28" s="7">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F28" s="2">
@@ -1437,7 +1450,7 @@
         <f>MATCH((A28-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H28" s="29">
+      <c r="H28" s="25">
         <f>MATCH(A28,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>125</v>
       </c>
@@ -1454,10 +1467,10 @@
       <c r="A29" s="1">
         <v>38475</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B29" s="38">
         <v>0.03</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D29" s="7">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F29" s="2">
@@ -1468,7 +1481,7 @@
         <f>MATCH((A29-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H29" s="29">
+      <c r="H29" s="25">
         <f>MATCH(A29,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>126</v>
       </c>
@@ -1485,10 +1498,10 @@
       <c r="A30" s="1">
         <v>38433</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30" s="38">
         <v>2.75E-2</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="7">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F30" s="2">
@@ -1499,7 +1512,7 @@
         <f>MATCH((A30-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H30" s="29">
+      <c r="H30" s="25">
         <f>MATCH(A30,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>127</v>
       </c>
@@ -1516,10 +1529,10 @@
       <c r="A31" s="1">
         <v>38385</v>
       </c>
-      <c r="B31" s="8">
+      <c r="B31" s="38">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D31" s="7">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F31" s="2">
@@ -1530,7 +1543,7 @@
         <f>MATCH((A31-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H31" s="29">
+      <c r="H31" s="25">
         <f>MATCH(A31,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>128</v>
       </c>
@@ -1547,10 +1560,10 @@
       <c r="A32" s="1">
         <v>38335</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B32" s="38">
         <v>2.2499999999999999E-2</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D32" s="7">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F32" s="2">
@@ -1561,7 +1574,7 @@
         <f>MATCH((A32-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H32" s="29">
+      <c r="H32" s="25">
         <f>MATCH(A32,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>129</v>
       </c>
@@ -1578,10 +1591,10 @@
       <c r="A33" s="1">
         <v>38301</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33" s="38">
         <v>0.02</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D33" s="7">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F33" s="2">
@@ -1592,7 +1605,7 @@
         <f>MATCH((A33-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H33" s="29">
+      <c r="H33" s="25">
         <f>MATCH(A33,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>130</v>
       </c>
@@ -1609,10 +1622,10 @@
       <c r="A34" s="1">
         <v>38251</v>
       </c>
-      <c r="B34" s="8">
+      <c r="B34" s="38">
         <v>1.7500000000000002E-2</v>
       </c>
-      <c r="D34" s="8">
+      <c r="D34" s="7">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F34" s="2">
@@ -1623,7 +1636,7 @@
         <f>MATCH((A34-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H34" s="29">
+      <c r="H34" s="25">
         <f>MATCH(A34,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>131</v>
       </c>
@@ -1640,10 +1653,10 @@
       <c r="A35" s="1">
         <v>38209</v>
       </c>
-      <c r="B35" s="8">
+      <c r="B35" s="38">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D35" s="7">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F35" s="2">
@@ -1654,7 +1667,7 @@
         <f>MATCH((A35-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H35" s="29">
+      <c r="H35" s="25">
         <f>MATCH(A35,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>132</v>
       </c>
@@ -1671,10 +1684,10 @@
       <c r="A36" s="1">
         <v>38168</v>
       </c>
-      <c r="B36" s="8">
+      <c r="B36" s="38">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="D36" s="8">
+      <c r="D36" s="7">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F36" s="2">
@@ -1685,7 +1698,7 @@
         <f>MATCH((A36-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H36" s="29">
+      <c r="H36" s="25">
         <f>MATCH(A36,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>133</v>
       </c>
@@ -1699,14 +1712,14 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="6">
+      <c r="A37" s="5">
         <v>37797</v>
       </c>
-      <c r="B37" s="7">
+      <c r="B37" s="37">
         <v>0.01</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="7">
+      <c r="C37" s="37"/>
+      <c r="D37" s="6">
         <v>-2.5000000000000001E-3</v>
       </c>
       <c r="F37" s="2">
@@ -1717,7 +1730,7 @@
         <f>MATCH((A37-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H37" s="29">
+      <c r="H37" s="25">
         <f>MATCH(A37,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>142</v>
       </c>
@@ -1731,14 +1744,14 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="6">
+      <c r="A38" s="5">
         <v>37566</v>
       </c>
-      <c r="B38" s="7">
+      <c r="B38" s="37">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="C38" s="13"/>
-      <c r="D38" s="7">
+      <c r="C38" s="37"/>
+      <c r="D38" s="6">
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F38" s="2">
@@ -1749,7 +1762,7 @@
         <f>MATCH((A38-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H38" s="29">
+      <c r="H38" s="25">
         <f>MATCH(A38,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>151</v>
       </c>
@@ -1763,14 +1776,14 @@
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="15">
+      <c r="A39" s="12">
         <v>37236</v>
       </c>
-      <c r="B39" s="16">
+      <c r="B39" s="39">
         <v>1.7500000000000002E-2</v>
       </c>
-      <c r="C39" s="17"/>
-      <c r="D39" s="16">
+      <c r="C39" s="39"/>
+      <c r="D39" s="13">
         <v>-2.5000000000000001E-3</v>
       </c>
       <c r="F39" s="2">
@@ -1781,7 +1794,7 @@
         <f>MATCH((A39-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H39" s="29">
+      <c r="H39" s="25">
         <f>MATCH(A39,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>158</v>
       </c>
@@ -1795,13 +1808,13 @@
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="5">
+      <c r="A40" s="4">
         <v>37201</v>
       </c>
-      <c r="B40" s="8">
+      <c r="B40" s="38">
         <v>0.02</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D40" s="3">
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F40" s="2">
@@ -1812,7 +1825,7 @@
         <f>MATCH((A40-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H40" s="29">
+      <c r="H40" s="25">
         <f>MATCH(A40,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>159</v>
       </c>
@@ -1826,13 +1839,13 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="5">
+      <c r="A41" s="4">
         <v>37166</v>
       </c>
-      <c r="B41" s="8">
+      <c r="B41" s="38">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D41" s="3">
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F41" s="2">
@@ -1843,7 +1856,7 @@
         <f>MATCH((A41-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H41" s="29">
+      <c r="H41" s="25">
         <f>MATCH(A41,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>160</v>
       </c>
@@ -1857,13 +1870,13 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
+      <c r="A42" s="4">
         <v>37151</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B42" s="38">
         <v>0.03</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D42" s="3">
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F42" s="2">
@@ -1874,7 +1887,7 @@
         <f>MATCH((A42-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H42" s="29">
+      <c r="H42" s="25">
         <f>MATCH(A42,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>161</v>
       </c>
@@ -1888,13 +1901,13 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="5">
+      <c r="A43" s="4">
         <v>37124</v>
       </c>
-      <c r="B43" s="8">
+      <c r="B43" s="38">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="D43" s="4">
+      <c r="D43" s="3">
         <v>-2.5000000000000001E-3</v>
       </c>
       <c r="F43" s="2">
@@ -1905,7 +1918,7 @@
         <f>MATCH((A43-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H43" s="29">
+      <c r="H43" s="25">
         <f>MATCH(A43,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>163</v>
       </c>
@@ -1919,13 +1932,13 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="5">
+      <c r="A44" s="4">
         <v>37069</v>
       </c>
-      <c r="B44" s="8">
+      <c r="B44" s="38">
         <v>3.7499999999999999E-2</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D44" s="3">
         <v>-2.5000000000000001E-3</v>
       </c>
       <c r="F44" s="2">
@@ -1936,7 +1949,7 @@
         <f>MATCH((A44-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H44" s="29">
+      <c r="H44" s="25">
         <f>MATCH(A44,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>164</v>
       </c>
@@ -1950,13 +1963,13 @@
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="5">
+      <c r="A45" s="4">
         <v>37026</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B45" s="38">
         <v>0.04</v>
       </c>
-      <c r="D45" s="4">
+      <c r="D45" s="3">
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F45" s="2">
@@ -1967,7 +1980,7 @@
         <f>MATCH((A45-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H45" s="29">
+      <c r="H45" s="25">
         <f>MATCH(A45,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>165</v>
       </c>
@@ -1981,14 +1994,13 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="5">
+      <c r="A46" s="4">
         <v>36999</v>
       </c>
-      <c r="B46" s="8">
+      <c r="B46" s="38">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="C46" s="2"/>
-      <c r="D46" s="4">
+      <c r="D46" s="3">
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F46" s="2">
@@ -1999,7 +2011,7 @@
         <f>MATCH((A46-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H46" s="29">
+      <c r="H46" s="25">
         <f>MATCH(A46,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>166</v>
       </c>
@@ -2013,14 +2025,13 @@
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="5">
+      <c r="A47" s="4">
         <v>36970</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B47" s="38">
         <v>0.05</v>
       </c>
-      <c r="C47" s="2"/>
-      <c r="D47" s="4">
+      <c r="D47" s="3">
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F47" s="2">
@@ -2031,7 +2042,7 @@
         <f>MATCH((A47-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H47" s="29">
+      <c r="H47" s="25">
         <f>MATCH(A47,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>168</v>
       </c>
@@ -2045,14 +2056,13 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="5">
+      <c r="A48" s="4">
         <v>36922</v>
       </c>
-      <c r="B48" s="8">
+      <c r="B48" s="38">
         <v>5.5E-2</v>
       </c>
-      <c r="C48" s="2"/>
-      <c r="D48" s="4">
+      <c r="D48" s="3">
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F48" s="2">
@@ -2063,7 +2073,7 @@
         <f>MATCH((A48-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H48" s="29">
+      <c r="H48" s="25">
         <f>MATCH(A48,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>169</v>
       </c>
@@ -2077,14 +2087,14 @@
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="15">
+      <c r="A49" s="12">
         <v>36894</v>
       </c>
-      <c r="B49" s="16">
+      <c r="B49" s="39">
         <v>0.06</v>
       </c>
-      <c r="C49" s="16"/>
-      <c r="D49" s="16">
+      <c r="C49" s="39"/>
+      <c r="D49" s="13">
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F49" s="2">
@@ -2095,7 +2105,7 @@
         <f>MATCH((A49-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H49" s="29">
+      <c r="H49" s="25">
         <f>MATCH(A49,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>170</v>
       </c>
@@ -2109,14 +2119,14 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="18">
+      <c r="A50" s="14">
         <v>36662</v>
       </c>
-      <c r="B50" s="10">
+      <c r="B50" s="36">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="C50" s="10"/>
-      <c r="D50" s="14">
+      <c r="C50" s="36"/>
+      <c r="D50" s="11">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F50" s="2">
@@ -2127,7 +2137,7 @@
         <f>MATCH((A50-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H50" s="29">
+      <c r="H50" s="25">
         <f>MATCH(A50,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>176</v>
       </c>
@@ -2144,11 +2154,10 @@
       <c r="A51" s="1">
         <v>36606</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="35">
         <v>0.06</v>
       </c>
-      <c r="C51" s="2"/>
-      <c r="D51" s="8">
+      <c r="D51" s="7">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F51" s="2">
@@ -2159,7 +2168,7 @@
         <f>MATCH((A51-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H51" s="29">
+      <c r="H51" s="25">
         <f>MATCH(A51,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>177</v>
       </c>
@@ -2176,11 +2185,10 @@
       <c r="A52" s="1">
         <v>36558</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B52" s="35">
         <v>5.7500000000000002E-2</v>
       </c>
-      <c r="C52" s="2"/>
-      <c r="D52" s="8">
+      <c r="D52" s="7">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F52" s="2">
@@ -2191,7 +2199,7 @@
         <f>MATCH((A52-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H52" s="29">
+      <c r="H52" s="25">
         <f>MATCH(A52,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>178</v>
       </c>
@@ -2208,11 +2216,10 @@
       <c r="A53" s="1">
         <v>36480</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" s="35">
         <v>5.5E-2</v>
       </c>
-      <c r="C53" s="2"/>
-      <c r="D53" s="8">
+      <c r="D53" s="7">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F53" s="2">
@@ -2223,7 +2230,7 @@
         <f>MATCH((A53-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H53" s="29">
+      <c r="H53" s="25">
         <f>MATCH(A53,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>180</v>
       </c>
@@ -2240,11 +2247,10 @@
       <c r="A54" s="1">
         <v>36396</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54" s="35">
         <v>5.2499999999999998E-2</v>
       </c>
-      <c r="C54" s="2"/>
-      <c r="D54" s="8">
+      <c r="D54" s="7">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F54" s="2">
@@ -2255,7 +2261,7 @@
         <f>MATCH((A54-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H54" s="29">
+      <c r="H54" s="25">
         <f>MATCH(A54,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>182</v>
       </c>
@@ -2272,11 +2278,10 @@
       <c r="A55" s="1">
         <v>36341</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55" s="35">
         <v>0.05</v>
       </c>
-      <c r="C55" s="2"/>
-      <c r="D55" s="8">
+      <c r="D55" s="7">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F55" s="2">
@@ -2287,7 +2292,7 @@
         <f>MATCH((A55-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H55" s="29">
+      <c r="H55" s="25">
         <f>MATCH(A55,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>183</v>
       </c>
@@ -2304,11 +2309,10 @@
       <c r="A56" s="1">
         <v>36116</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B56" s="35">
         <v>4.7500000000000001E-2</v>
       </c>
-      <c r="C56" s="2"/>
-      <c r="D56" s="8">
+      <c r="D56" s="7">
         <v>-2.5000000000000001E-3</v>
       </c>
       <c r="F56" s="2">
@@ -2319,7 +2323,7 @@
         <f>MATCH((A56-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H56" s="29">
+      <c r="H56" s="25">
         <f>MATCH(A56,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>188</v>
       </c>
@@ -2336,11 +2340,10 @@
       <c r="A57" s="1">
         <v>36083</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B57" s="35">
         <v>0.05</v>
       </c>
-      <c r="C57" s="2"/>
-      <c r="D57" s="8">
+      <c r="D57" s="7">
         <v>-2.5000000000000001E-3</v>
       </c>
       <c r="F57" s="2">
@@ -2351,7 +2354,7 @@
         <f>MATCH((A57-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H57" s="29">
+      <c r="H57" s="25">
         <f>MATCH(A57,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>189</v>
       </c>
@@ -2368,18 +2371,17 @@
       <c r="A58" s="1">
         <v>36067</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58" s="35">
         <v>5.2499999999999998E-2</v>
       </c>
-      <c r="C58" s="2"/>
-      <c r="D58" s="8">
+      <c r="D58" s="7">
         <v>-2.5000000000000001E-3</v>
       </c>
       <c r="G58" t="e">
         <f>MATCH((A58-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H58" s="29">
+      <c r="H58" s="25">
         <f>MATCH(A58,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>190</v>
       </c>
@@ -2393,8 +2395,6 @@
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
   </sheetData>
@@ -2407,8 +2407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96504E55-3F76-42FC-885A-83EA18AD498E}">
   <dimension ref="A1:D197"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H193" sqref="H193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2431,1276 +2431,1276 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20">
+    <row r="2" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16">
         <v>43369</v>
       </c>
-      <c r="B2" s="21">
-        <v>1</v>
-      </c>
-      <c r="D2" s="21" t="s">
+      <c r="B2" s="17">
+        <v>1</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20">
+    <row r="3" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
         <v>43313</v>
       </c>
-      <c r="B3" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20">
+      <c r="B3" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
         <v>43264</v>
       </c>
-      <c r="B4" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20">
+      <c r="B4" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
         <v>43222</v>
       </c>
-      <c r="B5" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20">
+      <c r="B5" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16">
         <v>43180</v>
       </c>
-      <c r="B6" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20">
+      <c r="B6" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
         <v>43131</v>
       </c>
-      <c r="B7" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22">
+      <c r="B7" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="18">
         <v>43082</v>
       </c>
-      <c r="B8" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
+      <c r="B8" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="18">
         <v>43040</v>
       </c>
-      <c r="B9" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22">
+      <c r="B9" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18">
         <v>42998</v>
       </c>
-      <c r="B10" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
+      <c r="B10" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="18">
         <v>42942</v>
       </c>
-      <c r="B11" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22">
+      <c r="B11" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18">
         <v>42900</v>
       </c>
-      <c r="B12" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22">
+      <c r="B12" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="18">
         <v>42858</v>
       </c>
-      <c r="B13" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22">
+      <c r="B13" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18">
         <v>42809</v>
       </c>
-      <c r="B14" s="23">
+      <c r="B14" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="22">
+      <c r="A15" s="18">
         <v>42767</v>
       </c>
-      <c r="B15" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20">
+      <c r="B15" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16">
         <v>42718</v>
       </c>
-      <c r="B16" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20">
+      <c r="B16" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16">
         <v>42676</v>
       </c>
-      <c r="B17" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20">
+      <c r="B17" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16">
         <v>42999</v>
       </c>
-      <c r="B18" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20">
+      <c r="B18" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="16">
         <v>42578</v>
       </c>
-      <c r="B19" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20">
+      <c r="B19" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16">
         <v>42536</v>
       </c>
-      <c r="B20" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20">
+      <c r="B20" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="16">
         <v>42487</v>
       </c>
-      <c r="B21" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="20">
+      <c r="B21" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="16">
         <v>42445</v>
       </c>
-      <c r="B22" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20">
+      <c r="B22" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="16">
         <v>42396</v>
       </c>
-      <c r="B23" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="22">
+      <c r="B23" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="18">
         <v>42354</v>
       </c>
-      <c r="B24" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22">
+      <c r="B24" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="18">
         <v>42305</v>
       </c>
-      <c r="B25" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22">
+      <c r="B25" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="18">
         <v>42264</v>
       </c>
-      <c r="B26" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="22">
+      <c r="B26" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="18">
         <v>42214</v>
       </c>
-      <c r="B27" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="22">
+      <c r="B27" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="18">
         <v>42172</v>
       </c>
-      <c r="B28" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="22">
+      <c r="B28" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="18">
         <v>42123</v>
       </c>
-      <c r="B29" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="22">
+      <c r="B29" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="18">
         <v>42081</v>
       </c>
-      <c r="B30" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="22">
+      <c r="B30" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="18">
         <v>42032</v>
       </c>
-      <c r="B31" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="20">
+      <c r="B31" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="16">
         <v>41990</v>
       </c>
-      <c r="B32" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="20">
+      <c r="B32" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="16">
         <v>41941</v>
       </c>
-      <c r="B33" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="20">
+      <c r="B33" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="16">
         <v>41899</v>
       </c>
-      <c r="B34" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="20">
+      <c r="B34" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="16">
         <v>41850</v>
       </c>
-      <c r="B35" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="20">
+      <c r="B35" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="16">
         <v>41808</v>
       </c>
-      <c r="B36" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="20">
+      <c r="B36" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="16">
         <v>41759</v>
       </c>
-      <c r="B37" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="20">
+      <c r="B37" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="16">
         <v>41717</v>
       </c>
-      <c r="B38" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="25">
+      <c r="B38" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="21">
         <v>41702</v>
       </c>
-      <c r="B39" s="26">
-        <v>0</v>
-      </c>
-      <c r="C39" s="26" t="s">
+      <c r="B39" s="22">
+        <v>0</v>
+      </c>
+      <c r="C39" s="22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="20">
+    <row r="40" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="16">
         <v>41668</v>
       </c>
-      <c r="B40" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="22">
+      <c r="B40" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="18">
         <v>41626</v>
       </c>
-      <c r="B41" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="22">
+      <c r="B41" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="18">
         <v>41577</v>
       </c>
-      <c r="B42" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="27">
+      <c r="B42" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="23">
         <v>41563</v>
       </c>
-      <c r="B43" s="24">
-        <v>0</v>
-      </c>
-      <c r="C43" s="24" t="s">
+      <c r="B43" s="20">
+        <v>0</v>
+      </c>
+      <c r="C43" s="20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="22">
+    <row r="44" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="18">
         <v>41535</v>
       </c>
-      <c r="B44" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="22">
+      <c r="B44" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="18">
         <v>41486</v>
       </c>
-      <c r="B45" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="22">
+      <c r="B45" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="18">
         <v>41444</v>
       </c>
-      <c r="B46" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="22">
+      <c r="B46" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="18">
         <v>41395</v>
       </c>
-      <c r="B47" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="22">
+      <c r="B47" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="18">
         <v>41353</v>
       </c>
-      <c r="B48" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="22">
+      <c r="B48" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="18">
         <v>41304</v>
       </c>
-      <c r="B49" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="20">
+      <c r="B49" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="16">
         <v>41255</v>
       </c>
-      <c r="B50" s="21">
-        <v>1</v>
-      </c>
-      <c r="D50" s="21" t="s">
+      <c r="B50" s="17">
+        <v>1</v>
+      </c>
+      <c r="D50" s="17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="20">
+    <row r="51" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="16">
         <v>41206</v>
       </c>
-      <c r="B51" s="21">
-        <v>0</v>
-      </c>
-      <c r="D51" s="21" t="s">
+      <c r="B51" s="17">
+        <v>0</v>
+      </c>
+      <c r="D51" s="17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="20">
+    <row r="52" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="16">
         <v>41165</v>
       </c>
-      <c r="B52" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="20">
+      <c r="B52" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="16">
         <v>41122</v>
       </c>
-      <c r="B53" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="20">
+      <c r="B53" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="16">
         <v>41080</v>
       </c>
-      <c r="B54" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="20">
+      <c r="B54" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="16">
         <v>41024</v>
       </c>
-      <c r="B55" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="20">
+      <c r="B55" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="16">
         <v>40981</v>
       </c>
-      <c r="B56" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="20">
+      <c r="B56" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="16">
         <v>40933</v>
       </c>
-      <c r="B57" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="22">
+      <c r="B57" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="18">
         <v>40890</v>
       </c>
-      <c r="B58" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="27">
+      <c r="B58" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="23">
         <v>40875</v>
       </c>
-      <c r="B59" s="24">
-        <v>0</v>
-      </c>
-      <c r="C59" s="24" t="s">
+      <c r="B59" s="20">
+        <v>0</v>
+      </c>
+      <c r="C59" s="20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="22">
+    <row r="60" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="18">
         <v>40849</v>
       </c>
-      <c r="B60" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="22">
+      <c r="B60" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="18">
         <v>40807</v>
       </c>
-      <c r="B61" s="23">
-        <v>0</v>
-      </c>
-      <c r="C61" s="23"/>
-    </row>
-    <row r="62" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="22">
+      <c r="B61" s="19">
+        <v>0</v>
+      </c>
+      <c r="C61" s="19"/>
+    </row>
+    <row r="62" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="18">
         <v>40764</v>
       </c>
-      <c r="B62" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="27">
+      <c r="B62" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="23">
         <v>40756</v>
       </c>
-      <c r="B63" s="24">
-        <v>0</v>
-      </c>
-      <c r="C63" s="24" t="s">
+      <c r="B63" s="20">
+        <v>0</v>
+      </c>
+      <c r="C63" s="20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="22">
+    <row r="64" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="18">
         <v>40716</v>
       </c>
-      <c r="B64" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="22">
+      <c r="B64" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="18">
         <v>40660</v>
       </c>
-      <c r="B65" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="22">
+      <c r="B65" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="18">
         <v>36965</v>
       </c>
-      <c r="B66" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="22">
+      <c r="B66" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="18">
         <v>40569</v>
       </c>
-      <c r="B67" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="20">
+      <c r="B67" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="16">
         <v>40526</v>
       </c>
     </row>
-    <row r="69" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="20">
+    <row r="69" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="16">
         <v>40485</v>
       </c>
     </row>
-    <row r="70" spans="1:3" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="25">
+    <row r="70" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="21">
         <v>40466</v>
       </c>
-      <c r="C70" s="26" t="s">
+      <c r="C70" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="20">
+    <row r="71" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="16">
         <v>40442</v>
       </c>
     </row>
-    <row r="72" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="20">
+    <row r="72" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="16">
         <v>40400</v>
       </c>
     </row>
-    <row r="73" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="20">
+    <row r="73" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="16">
         <v>40352</v>
       </c>
     </row>
-    <row r="74" spans="1:3" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="25">
+    <row r="74" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="21">
         <v>40307</v>
       </c>
-      <c r="C74" s="26" t="s">
+      <c r="C74" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="20">
+    <row r="75" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="16">
         <v>40296</v>
       </c>
     </row>
-    <row r="76" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="20">
+    <row r="76" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="16">
         <v>40253</v>
       </c>
     </row>
-    <row r="77" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="20">
+    <row r="77" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="16">
         <v>40205</v>
       </c>
     </row>
-    <row r="78" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="22">
+    <row r="78" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="18">
         <v>40163</v>
       </c>
     </row>
-    <row r="79" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="22">
+    <row r="79" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="18">
         <v>40121</v>
       </c>
     </row>
-    <row r="80" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="22">
+    <row r="80" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="18">
         <v>40079</v>
       </c>
     </row>
-    <row r="81" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="22">
+    <row r="81" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="18">
         <v>40037</v>
       </c>
     </row>
-    <row r="82" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="22">
+    <row r="82" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="18">
         <v>39988</v>
       </c>
     </row>
-    <row r="83" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="27">
+    <row r="83" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="23">
         <v>39967</v>
       </c>
-      <c r="C83" s="24" t="s">
+      <c r="C83" s="20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="22">
+    <row r="84" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="18">
         <v>39932</v>
       </c>
     </row>
-    <row r="85" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="22">
+    <row r="85" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="18">
         <v>39890</v>
       </c>
     </row>
-    <row r="86" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="22">
+    <row r="86" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="18">
         <v>39851</v>
       </c>
     </row>
-    <row r="87" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="22">
-        <v>39815</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="27">
+    <row r="87" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="18">
+        <v>39841</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="23">
         <v>39829</v>
       </c>
-      <c r="C88" s="24" t="s">
+      <c r="C88" s="20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="30">
+    <row r="89" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="26">
         <v>39798</v>
       </c>
     </row>
-    <row r="90" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="30">
+    <row r="90" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="26">
         <v>39750</v>
       </c>
     </row>
-    <row r="91" spans="1:3" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="25">
+    <row r="91" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="21">
         <v>39728</v>
       </c>
-      <c r="C91" s="26" t="s">
+      <c r="C91" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:3" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="25">
+    <row r="92" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="21">
         <v>39720</v>
       </c>
-      <c r="C92" s="26" t="s">
+      <c r="C92" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="20">
+    <row r="93" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="16">
         <v>39707</v>
       </c>
     </row>
-    <row r="94" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="20">
+    <row r="94" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="16">
         <v>39665</v>
       </c>
     </row>
-    <row r="95" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="20">
+    <row r="95" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="16">
         <v>39653</v>
       </c>
     </row>
-    <row r="96" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="20">
+    <row r="96" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="16">
         <v>39624</v>
       </c>
     </row>
-    <row r="97" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="30">
+    <row r="97" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="26">
         <v>39568</v>
       </c>
     </row>
-    <row r="98" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="30">
+    <row r="98" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="26">
         <v>39525</v>
       </c>
     </row>
-    <row r="99" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="20">
+    <row r="99" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="16">
         <v>39517</v>
       </c>
     </row>
-    <row r="100" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="30">
+    <row r="100" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="26">
         <v>39477</v>
       </c>
     </row>
-    <row r="101" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="20">
+    <row r="101" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="16">
         <v>39468</v>
       </c>
     </row>
-    <row r="102" spans="1:3" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="25">
+    <row r="102" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="21">
         <v>39456</v>
       </c>
-      <c r="C102" s="26" t="s">
+      <c r="C102" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:3" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="34">
+    <row r="103" spans="1:3" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="30">
         <v>39427</v>
       </c>
     </row>
-    <row r="104" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="27">
+    <row r="104" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="23">
         <v>39422</v>
       </c>
-      <c r="C104" s="24" t="s">
+      <c r="C104" s="20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:3" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="34">
+    <row r="105" spans="1:3" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="30">
         <v>39386</v>
       </c>
     </row>
-    <row r="106" spans="1:3" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="34">
+    <row r="106" spans="1:3" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="30">
         <v>39343</v>
       </c>
     </row>
-    <row r="107" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="31">
+    <row r="107" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="27">
         <v>39310</v>
       </c>
-      <c r="B107" s="12"/>
-      <c r="C107" s="12" t="s">
+      <c r="B107" s="10"/>
+      <c r="C107" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="31">
+    <row r="108" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="27">
         <v>39304</v>
       </c>
-      <c r="B108" s="12"/>
-      <c r="C108" s="12" t="s">
+      <c r="B108" s="10"/>
+      <c r="C108" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="109" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="32">
+    <row r="109" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="28">
         <v>39301</v>
       </c>
-      <c r="B109" s="33"/>
-      <c r="C109" s="33"/>
-    </row>
-    <row r="110" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="22">
+      <c r="B109" s="29"/>
+      <c r="C109" s="29"/>
+    </row>
+    <row r="110" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="18">
         <v>39261</v>
       </c>
     </row>
-    <row r="111" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="22">
+    <row r="111" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="18">
         <v>39211</v>
       </c>
     </row>
-    <row r="112" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="22">
+    <row r="112" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="18">
         <v>39162</v>
       </c>
     </row>
-    <row r="113" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="22">
+    <row r="113" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="18">
         <v>39113</v>
       </c>
     </row>
-    <row r="114" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="20">
+    <row r="114" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="16">
         <v>39063</v>
       </c>
     </row>
-    <row r="115" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="20">
+    <row r="115" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="16">
         <v>39015</v>
       </c>
     </row>
-    <row r="116" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="20">
+    <row r="116" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="16">
         <v>38980</v>
       </c>
     </row>
-    <row r="117" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="20">
+    <row r="117" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="16">
         <v>38937</v>
       </c>
     </row>
-    <row r="118" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="20">
+    <row r="118" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="16">
         <v>38897</v>
       </c>
     </row>
-    <row r="119" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="20">
+    <row r="119" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="16">
         <v>38847</v>
       </c>
     </row>
-    <row r="120" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="20">
+    <row r="120" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="16">
         <v>38804</v>
       </c>
     </row>
-    <row r="121" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="20">
+    <row r="121" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="16">
         <v>38748</v>
       </c>
     </row>
-    <row r="122" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="22">
+    <row r="122" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="18">
         <v>38699</v>
       </c>
     </row>
-    <row r="123" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="22">
+    <row r="123" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="18">
         <v>38657</v>
       </c>
     </row>
-    <row r="124" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="22">
+    <row r="124" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="18">
         <v>38615</v>
       </c>
     </row>
-    <row r="125" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="22">
+    <row r="125" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="18">
         <v>38573</v>
       </c>
     </row>
-    <row r="126" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="22">
+    <row r="126" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="18">
         <v>38533</v>
       </c>
     </row>
-    <row r="127" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="22">
+    <row r="127" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="18">
         <v>38475</v>
       </c>
     </row>
-    <row r="128" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="22">
+    <row r="128" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="18">
         <v>38433</v>
       </c>
     </row>
-    <row r="129" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="22">
+    <row r="129" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="18">
         <v>38385</v>
       </c>
     </row>
-    <row r="130" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="20">
+    <row r="130" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="16">
         <v>38335</v>
       </c>
     </row>
-    <row r="131" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="20">
+    <row r="131" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="16">
         <v>38301</v>
       </c>
     </row>
-    <row r="132" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="20">
+    <row r="132" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="16">
         <v>38251</v>
       </c>
     </row>
-    <row r="133" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="20">
+    <row r="133" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="16">
         <v>38209</v>
       </c>
     </row>
-    <row r="134" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="20">
+    <row r="134" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="16">
         <v>38168</v>
       </c>
     </row>
-    <row r="135" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="20">
+    <row r="135" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="16">
         <v>38111</v>
       </c>
     </row>
-    <row r="136" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="20">
+    <row r="136" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="16">
         <v>38062</v>
       </c>
     </row>
-    <row r="137" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="20">
+    <row r="137" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="16">
         <v>38014</v>
       </c>
     </row>
-    <row r="138" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="22">
+    <row r="138" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="18">
         <v>37964</v>
       </c>
     </row>
-    <row r="139" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="22">
+    <row r="139" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="18">
         <v>37922</v>
       </c>
     </row>
-    <row r="140" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="22">
+    <row r="140" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="18">
         <v>37880</v>
       </c>
     </row>
-    <row r="141" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="22">
+    <row r="141" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="18">
         <v>37879</v>
       </c>
     </row>
-    <row r="142" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="22">
+    <row r="142" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="18">
         <v>37845</v>
       </c>
     </row>
-    <row r="143" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="22">
+    <row r="143" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="18">
         <v>37797</v>
       </c>
     </row>
-    <row r="144" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="22">
+    <row r="144" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="18">
         <v>37747</v>
       </c>
     </row>
-    <row r="145" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="27">
+    <row r="145" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="23">
         <v>37727</v>
       </c>
-      <c r="C145" s="24" t="s">
+      <c r="C145" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="146" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="27">
+    <row r="146" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="23">
         <v>37719</v>
       </c>
-      <c r="C146" s="24" t="s">
+      <c r="C146" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="147" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="27">
+    <row r="147" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="23">
         <v>37712</v>
       </c>
-      <c r="C147" s="24" t="s">
+      <c r="C147" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="148" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="27">
+    <row r="148" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="23">
         <v>37705</v>
       </c>
-      <c r="C148" s="24" t="s">
+      <c r="C148" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="149" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="22">
+    <row r="149" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="18">
         <v>37698</v>
       </c>
     </row>
-    <row r="150" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="22">
+    <row r="150" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="18">
         <v>37650</v>
       </c>
     </row>
-    <row r="151" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="20">
+    <row r="151" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="16">
         <v>37600</v>
       </c>
     </row>
-    <row r="152" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="20">
+    <row r="152" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="16">
         <v>37566</v>
       </c>
     </row>
-    <row r="153" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="20">
+    <row r="153" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="16">
         <v>37523</v>
       </c>
     </row>
-    <row r="154" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="20">
+    <row r="154" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="16">
         <v>37481</v>
       </c>
     </row>
-    <row r="155" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="20">
+    <row r="155" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="16">
         <v>37433</v>
       </c>
     </row>
-    <row r="156" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="20">
+    <row r="156" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="16">
         <v>37383</v>
       </c>
     </row>
-    <row r="157" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="20">
+    <row r="157" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="16">
         <v>37334</v>
       </c>
     </row>
-    <row r="158" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="20">
+    <row r="158" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="16">
         <v>37286</v>
       </c>
     </row>
-    <row r="159" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="22">
+    <row r="159" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="18">
         <v>37236</v>
       </c>
     </row>
-    <row r="160" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="22">
+    <row r="160" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="18">
         <v>37201</v>
       </c>
     </row>
-    <row r="161" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="22">
+    <row r="161" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="18">
         <v>37166</v>
       </c>
     </row>
-    <row r="162" spans="1:3" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="36">
+    <row r="162" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="32">
         <v>37151</v>
       </c>
-      <c r="B162" s="37"/>
-      <c r="C162" s="37" t="s">
+      <c r="B162" s="33"/>
+      <c r="C162" s="33" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="163" spans="1:3" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="36">
+    <row r="163" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="32">
         <v>37147</v>
       </c>
-      <c r="B163" s="37"/>
-      <c r="C163" s="37" t="s">
+      <c r="B163" s="33"/>
+      <c r="C163" s="33" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="164" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="22">
+    <row r="164" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="18">
         <v>37124</v>
       </c>
     </row>
-    <row r="165" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="22">
+    <row r="165" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="18">
         <v>37069</v>
       </c>
     </row>
-    <row r="166" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="22">
+    <row r="166" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="18">
         <v>37026</v>
       </c>
     </row>
-    <row r="167" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="27">
+    <row r="167" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="23">
         <v>36999</v>
       </c>
-      <c r="B167" s="24"/>
-      <c r="C167" s="24" t="s">
+      <c r="B167" s="20"/>
+      <c r="C167" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="168" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="27">
+    <row r="168" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="23">
         <v>36992</v>
       </c>
-      <c r="B168" s="24"/>
-      <c r="C168" s="24" t="s">
+      <c r="B168" s="20"/>
+      <c r="C168" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="169" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="22">
+    <row r="169" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="18">
         <v>36970</v>
       </c>
     </row>
-    <row r="170" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="22">
+    <row r="170" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="18">
         <v>36922</v>
       </c>
     </row>
-    <row r="171" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="27">
+    <row r="171" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="23">
         <v>36894</v>
       </c>
-      <c r="B171" s="24"/>
-      <c r="C171" s="24" t="s">
+      <c r="B171" s="20"/>
+      <c r="C171" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="172" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="20">
+    <row r="172" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="16">
         <v>36879</v>
       </c>
     </row>
-    <row r="173" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="20">
+    <row r="173" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="16">
         <v>36845</v>
       </c>
     </row>
-    <row r="174" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="20">
+    <row r="174" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="16">
         <v>36802</v>
       </c>
     </row>
-    <row r="175" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="20">
+    <row r="175" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="16">
         <v>36760</v>
       </c>
     </row>
-    <row r="176" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="20">
+    <row r="176" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="16">
         <v>36705</v>
       </c>
     </row>
-    <row r="177" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="20">
+    <row r="177" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="16">
         <v>36662</v>
       </c>
     </row>
-    <row r="178" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="20">
+    <row r="178" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="16">
         <v>36606</v>
       </c>
     </row>
-    <row r="179" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="20">
+    <row r="179" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="16">
         <v>36558</v>
       </c>
     </row>
-    <row r="180" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="22">
+    <row r="180" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A180" s="18">
         <v>36515</v>
       </c>
     </row>
-    <row r="181" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="22">
+    <row r="181" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="18">
         <v>36480</v>
       </c>
     </row>
-    <row r="182" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="22">
+    <row r="182" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="18">
         <v>36438</v>
       </c>
     </row>
-    <row r="183" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="22">
+    <row r="183" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="18">
         <v>36396</v>
       </c>
     </row>
-    <row r="184" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="22">
+    <row r="184" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="18">
         <v>36341</v>
       </c>
     </row>
-    <row r="185" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="22">
+    <row r="185" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="18">
         <v>36298</v>
       </c>
     </row>
-    <row r="186" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="22">
+    <row r="186" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="18">
         <v>36249</v>
       </c>
     </row>
-    <row r="187" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="22">
+    <row r="187" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="18">
         <v>36194</v>
       </c>
     </row>
-    <row r="188" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="20">
+    <row r="188" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="16">
         <v>36151</v>
       </c>
     </row>
-    <row r="189" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="20">
+    <row r="189" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A189" s="16">
         <v>36116</v>
       </c>
     </row>
-    <row r="190" spans="1:3" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="25">
+    <row r="190" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="21">
         <v>36083</v>
       </c>
-      <c r="C190" s="26" t="s">
+      <c r="C190" s="22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="191" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="20">
+    <row r="191" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="16">
         <v>36067</v>
       </c>
     </row>
-    <row r="192" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="25">
+    <row r="192" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="21">
         <v>36059</v>
       </c>
-      <c r="B192" s="26"/>
-      <c r="C192" s="26" t="s">
+      <c r="B192" s="22"/>
+      <c r="C192" s="22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="193" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="20">
+    <row r="193" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="16">
         <v>36025</v>
       </c>
     </row>
-    <row r="194" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="20">
+    <row r="194" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="16">
         <v>35977</v>
       </c>
     </row>
-    <row r="195" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="20">
+    <row r="195" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="16">
         <v>35934</v>
       </c>
     </row>
-    <row r="196" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="20">
+    <row r="196" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="16">
         <v>35885</v>
       </c>
     </row>
-    <row r="197" spans="1:1" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="20">
+    <row r="197" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A197" s="16">
         <v>35830</v>
       </c>
     </row>

</xml_diff>

<commit_message>
started collecting financial data, generated first tables for Latex
</commit_message>
<xml_diff>
--- a/TgtRateAdjustments.xlsx
+++ b/TgtRateAdjustments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\corin\Documents\Uni\M.A.HSG\MA_Arbeit\MasterThesis_NarrativesInFinance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721A5F0E-BF01-4D4A-9D58-F5AA1856EF95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923558EF-7F31-4A4F-A5CD-53DEE4A68E61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{80B993A4-3DA7-4240-872A-2188DEF1878B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{80B993A4-3DA7-4240-872A-2188DEF1878B}"/>
   </bookViews>
   <sheets>
     <sheet name="TgtRateAdjustment" sheetId="1" r:id="rId1"/>
@@ -120,7 +120,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,6 +175,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -189,7 +195,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -230,6 +236,10 @@
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E32174-ACCF-4909-B52B-590BE0998F4D}">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,6 +636,10 @@
         <f>IF(ISNA(H2),0,1)</f>
         <v>0</v>
       </c>
+      <c r="K2">
+        <f>D2*10000</f>
+        <v>25</v>
+      </c>
       <c r="M2" t="s">
         <v>18</v>
       </c>
@@ -663,6 +677,10 @@
         <f t="shared" ref="J3:J58" si="2">IF(ISNA(H3),0,1)</f>
         <v>0</v>
       </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K58" si="3">D3*10000</f>
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -697,6 +715,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="K4">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -731,6 +753,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="K5">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -765,6 +791,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="K6">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -799,6 +829,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="K7">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -833,6 +867,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="K8">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -867,6 +905,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="K9">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
@@ -904,6 +946,14 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
+      <c r="K10">
+        <f t="shared" si="3"/>
+        <v>-75</v>
+      </c>
+      <c r="L10">
+        <f t="shared" ref="L3:L10" si="4">E10*10000</f>
+        <v>-100</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -935,6 +985,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
+      <c r="K11">
+        <f t="shared" si="3"/>
+        <v>-50</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
@@ -966,6 +1020,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="K12">
+        <f t="shared" si="3"/>
+        <v>-50</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
@@ -997,6 +1055,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
+      <c r="K13">
+        <f t="shared" si="3"/>
+        <v>-25</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
@@ -1028,6 +1090,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
+      <c r="K14">
+        <f t="shared" si="3"/>
+        <v>-75</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
@@ -1059,6 +1125,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
+      <c r="K15">
+        <f t="shared" si="3"/>
+        <v>-50</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
@@ -1090,8 +1160,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <f t="shared" si="3"/>
+        <v>-75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>39427</v>
       </c>
@@ -1121,8 +1195,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17">
+        <f t="shared" si="3"/>
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>39386</v>
       </c>
@@ -1152,8 +1230,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18">
+        <f t="shared" si="3"/>
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>39343</v>
       </c>
@@ -1183,8 +1265,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19">
+        <f t="shared" si="3"/>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>38897</v>
       </c>
@@ -1214,8 +1300,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>38847</v>
       </c>
@@ -1245,8 +1335,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>38804</v>
       </c>
@@ -1276,8 +1370,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>38748</v>
       </c>
@@ -1307,8 +1405,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>38699</v>
       </c>
@@ -1338,8 +1440,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>38657</v>
       </c>
@@ -1369,8 +1475,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>38615</v>
       </c>
@@ -1400,8 +1510,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>38573</v>
       </c>
@@ -1412,7 +1526,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F27" s="2">
-        <f t="shared" ref="F27:F56" si="3">B28+D27-B27</f>
+        <f t="shared" ref="F27:F56" si="5">B28+D27-B27</f>
         <v>0</v>
       </c>
       <c r="G27" t="e">
@@ -1431,8 +1545,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>38533</v>
       </c>
@@ -1443,7 +1561,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F28" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G28" t="e">
@@ -1462,8 +1580,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>38475</v>
       </c>
@@ -1474,7 +1596,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F29" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G29" t="e">
@@ -1493,8 +1615,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>38433</v>
       </c>
@@ -1505,7 +1631,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F30" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G30" t="e">
@@ -1524,39 +1650,48 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+      <c r="K30">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="40">
         <v>38385</v>
       </c>
-      <c r="B31" s="38">
+      <c r="B31" s="41">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D31" s="7">
+      <c r="C31" s="41"/>
+      <c r="D31" s="42">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="F31" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G31" t="e">
+      <c r="F31" s="42">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G31" s="43" t="e">
         <f>MATCH((A31-1), FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="H31" s="25">
+      <c r="H31" s="43">
         <f>MATCH(A31,FOMC_Meetings!$A$2:$A$197,0)</f>
         <v>128</v>
       </c>
-      <c r="I31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J31">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I31" s="43">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J31" s="43">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K31" s="43">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>38335</v>
       </c>
@@ -1567,7 +1702,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F32" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G32" t="e">
@@ -1586,8 +1721,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>38301</v>
       </c>
@@ -1598,7 +1737,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F33" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G33" t="e">
@@ -1617,8 +1756,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>38251</v>
       </c>
@@ -1629,7 +1772,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F34" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G34" t="e">
@@ -1648,8 +1791,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K34">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>38209</v>
       </c>
@@ -1660,7 +1807,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F35" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G35" t="e">
@@ -1679,8 +1826,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K35">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>38168</v>
       </c>
@@ -1691,7 +1842,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F36" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G36" t="e">
@@ -1710,8 +1861,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K36">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>37797</v>
       </c>
@@ -1742,8 +1897,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K37">
+        <f t="shared" si="3"/>
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>37566</v>
       </c>
@@ -1755,7 +1914,7 @@
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F38" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G38" t="e">
@@ -1774,8 +1933,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K38">
+        <f t="shared" si="3"/>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <v>37236</v>
       </c>
@@ -1787,7 +1950,7 @@
         <v>-2.5000000000000001E-3</v>
       </c>
       <c r="F39" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G39" t="e">
@@ -1806,8 +1969,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K39">
+        <f t="shared" si="3"/>
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>37201</v>
       </c>
@@ -1818,7 +1985,7 @@
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F40" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G40" t="e">
@@ -1837,8 +2004,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K40">
+        <f t="shared" si="3"/>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>37166</v>
       </c>
@@ -1849,7 +2020,7 @@
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F41" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G41" t="e">
@@ -1868,8 +2039,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K41">
+        <f t="shared" si="3"/>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>37151</v>
       </c>
@@ -1880,7 +2055,7 @@
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F42" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G42" t="e">
@@ -1899,8 +2074,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K42">
+        <f t="shared" si="3"/>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>37124</v>
       </c>
@@ -1911,7 +2090,7 @@
         <v>-2.5000000000000001E-3</v>
       </c>
       <c r="F43" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G43" t="e">
@@ -1930,8 +2109,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K43">
+        <f t="shared" si="3"/>
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>37069</v>
       </c>
@@ -1942,7 +2125,7 @@
         <v>-2.5000000000000001E-3</v>
       </c>
       <c r="F44" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G44" t="e">
@@ -1961,8 +2144,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K44">
+        <f t="shared" si="3"/>
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>37026</v>
       </c>
@@ -1973,7 +2160,7 @@
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F45" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G45" t="e">
@@ -1992,8 +2179,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K45">
+        <f t="shared" si="3"/>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>36999</v>
       </c>
@@ -2004,7 +2195,7 @@
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F46" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G46" t="e">
@@ -2023,8 +2214,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K46">
+        <f t="shared" si="3"/>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>36970</v>
       </c>
@@ -2035,7 +2230,7 @@
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F47" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G47" t="e">
@@ -2054,8 +2249,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K47">
+        <f t="shared" si="3"/>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>36922</v>
       </c>
@@ -2066,7 +2265,7 @@
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F48" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G48" t="e">
@@ -2085,8 +2284,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K48">
+        <f t="shared" si="3"/>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="12">
         <v>36894</v>
       </c>
@@ -2098,7 +2301,7 @@
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F49" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G49" t="e">
@@ -2117,8 +2320,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K49">
+        <f t="shared" si="3"/>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="14">
         <v>36662</v>
       </c>
@@ -2130,7 +2337,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F50" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G50" t="e">
@@ -2149,8 +2356,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K50">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>36606</v>
       </c>
@@ -2161,7 +2372,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F51" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G51" t="e">
@@ -2180,8 +2391,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K51">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>36558</v>
       </c>
@@ -2192,7 +2407,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F52" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G52" t="e">
@@ -2211,8 +2426,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K52">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>36480</v>
       </c>
@@ -2223,7 +2442,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F53" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G53" t="e">
@@ -2242,8 +2461,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K53">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>36396</v>
       </c>
@@ -2254,7 +2477,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F54" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G54" t="e">
@@ -2273,8 +2496,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K54">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>36341</v>
       </c>
@@ -2285,7 +2512,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F55" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G55" t="e">
@@ -2304,8 +2531,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K55">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>36116</v>
       </c>
@@ -2316,7 +2547,7 @@
         <v>-2.5000000000000001E-3</v>
       </c>
       <c r="F56" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G56" t="e">
@@ -2335,8 +2566,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K56">
+        <f t="shared" si="3"/>
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>36083</v>
       </c>
@@ -2366,8 +2601,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K57">
+        <f t="shared" si="3"/>
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>36067</v>
       </c>
@@ -2393,8 +2632,12 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K58">
+        <f t="shared" si="3"/>
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D59" s="2"/>
     </row>
   </sheetData>
@@ -2407,8 +2650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96504E55-3F76-42FC-885A-83EA18AD498E}">
   <dimension ref="A1:D197"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H193" sqref="H193"/>
+    <sheetView topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="A170" sqref="A170:A197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2650,11 +2893,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="18">
+    <row r="29" spans="1:2" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="28">
         <v>42123</v>
       </c>
-      <c r="B29" s="19">
+      <c r="B29" s="29">
         <v>0</v>
       </c>
     </row>
@@ -2816,7 +3059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="18">
         <v>41304</v>
       </c>
@@ -2886,11 +3129,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="16">
+    <row r="57" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="28">
         <v>40933</v>
       </c>
-      <c r="B57" s="17">
+      <c r="B57" s="29">
         <v>1</v>
       </c>
     </row>
@@ -3075,8 +3318,8 @@
         <v>39932</v>
       </c>
     </row>
-    <row r="85" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="18">
+    <row r="85" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="28">
         <v>39890</v>
       </c>
     </row>
@@ -3240,8 +3483,8 @@
         <v>39162</v>
       </c>
     </row>
-    <row r="113" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="18">
+    <row r="113" spans="1:1" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="28">
         <v>39113</v>
       </c>
     </row>
@@ -3380,8 +3623,8 @@
         <v>37880</v>
       </c>
     </row>
-    <row r="141" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="18">
+    <row r="141" spans="1:1" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="28">
         <v>37879</v>
       </c>
     </row>
@@ -3548,8 +3791,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="169" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="18">
+    <row r="169" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="28">
         <v>36970</v>
       </c>
     </row>

</xml_diff>

<commit_message>
worked on FOMC data, added text in Chapter 5 and adjusted tables
</commit_message>
<xml_diff>
--- a/TgtRateAdjustments.xlsx
+++ b/TgtRateAdjustments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\corin\Documents\Uni\M.A.HSG\MA_Arbeit\MasterThesis_NarrativesInFinance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923558EF-7F31-4A4F-A5CD-53DEE4A68E61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41CDFA6-4A45-4E76-AB09-9A9A9FF442EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{80B993A4-3DA7-4240-872A-2188DEF1878B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -89,6 +89,12 @@
   <si>
     <t>https://www.federalreserve.gov/monetarypolicy/openmarket.htm</t>
   </si>
+  <si>
+    <t>Meeting am 15.09. gelöscht, da wohl zu 16.09.gehört</t>
+  </si>
+  <si>
+    <t>Meeting unscheduled</t>
+  </si>
 </sst>
 </file>
 
@@ -120,7 +126,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,6 +187,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -195,7 +207,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -240,6 +252,12 @@
     <xf numFmtId="10" fontId="0" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,7 +576,7 @@
   <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="A58" sqref="A2:A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,6 +587,7 @@
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="11" max="11" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -599,6 +618,9 @@
       <c r="J1" t="s">
         <v>15</v>
       </c>
+      <c r="K1" s="43" t="s">
+        <v>20</v>
+      </c>
       <c r="M1" t="s">
         <v>17</v>
       </c>
@@ -621,11 +643,11 @@
         <v>0</v>
       </c>
       <c r="G2" s="25">
-        <f>MATCH((A2-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A2-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>1</v>
       </c>
       <c r="H2" t="e">
-        <f>MATCH(A2,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A2,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="I2">
@@ -637,8 +659,8 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <f>D2*10000</f>
-        <v>25</v>
+        <f>VLOOKUP(IF(I2=1,(A2-1),A2),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
       <c r="M2" t="s">
         <v>18</v>
@@ -662,11 +684,11 @@
         <v>0</v>
       </c>
       <c r="G3" s="25">
-        <f>MATCH((A3-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A3-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>3</v>
       </c>
       <c r="H3" t="e">
-        <f>MATCH(A3,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A3,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="I3">
@@ -678,8 +700,8 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K58" si="3">D3*10000</f>
-        <v>25</v>
+        <f>VLOOKUP(IF(I3=1,(A3-1),A3),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -700,11 +722,11 @@
         <v>0</v>
       </c>
       <c r="G4" s="25">
-        <f>MATCH((A4-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A4-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>5</v>
       </c>
       <c r="H4" t="e">
-        <f>MATCH(A4,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A4,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="I4">
@@ -716,8 +738,8 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I4=1,(A4-1),A4),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -738,11 +760,11 @@
         <v>0</v>
       </c>
       <c r="G5" s="25">
-        <f>MATCH((A5-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A5-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>7</v>
       </c>
       <c r="H5" t="e">
-        <f>MATCH(A5,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A5,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="I5">
@@ -754,8 +776,8 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I5=1,(A5-1),A5),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -776,11 +798,11 @@
         <v>0</v>
       </c>
       <c r="G6" s="25">
-        <f>MATCH((A6-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A6-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>11</v>
       </c>
       <c r="H6" t="e">
-        <f>MATCH(A6,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A6,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="I6">
@@ -792,8 +814,8 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I6=1,(A6-1),A6),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -814,11 +836,11 @@
         <v>0</v>
       </c>
       <c r="G7" s="25">
-        <f>MATCH((A7-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A7-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>13</v>
       </c>
       <c r="H7" t="e">
-        <f>MATCH(A7,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A7,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="I7">
@@ -830,8 +852,8 @@
         <v>0</v>
       </c>
       <c r="K7">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I7=1,(A7-1),A7),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -852,11 +874,11 @@
         <v>0</v>
       </c>
       <c r="G8" s="25">
-        <f>MATCH((A8-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A8-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>15</v>
       </c>
       <c r="H8" t="e">
-        <f>MATCH(A8,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A8,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="I8">
@@ -868,8 +890,8 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I8=1,(A8-1),A8),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -890,11 +912,11 @@
         <v>0</v>
       </c>
       <c r="G9" s="25">
-        <f>MATCH((A9-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A9-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>23</v>
       </c>
       <c r="H9" t="e">
-        <f>MATCH(A9,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A9,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="I9">
@@ -906,8 +928,8 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I9=1,(A9-1),A9),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -931,11 +953,11 @@
         <v>2.5000000000000005E-3</v>
       </c>
       <c r="G10" t="e">
-        <f>MATCH((A10-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A10-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H10" s="25">
-        <f>MATCH(A10,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A10,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>88</v>
       </c>
       <c r="I10">
@@ -947,12 +969,8 @@
         <v>1</v>
       </c>
       <c r="K10">
-        <f t="shared" si="3"/>
-        <v>-75</v>
-      </c>
-      <c r="L10">
-        <f t="shared" ref="L3:L10" si="4">E10*10000</f>
-        <v>-100</v>
+        <f>VLOOKUP(IF(I10=1,(A10-1),A10),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -970,11 +988,11 @@
         <v>0</v>
       </c>
       <c r="G11" t="e">
-        <f>MATCH((A11-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A11-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H11" s="25">
-        <f>MATCH(A11,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A11,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>89</v>
       </c>
       <c r="I11">
@@ -986,43 +1004,44 @@
         <v>1</v>
       </c>
       <c r="K11">
-        <f t="shared" si="3"/>
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+        <f>VLOOKUP(IF(I11=1,(A11-1),A11),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="46">
         <v>39729</v>
       </c>
-      <c r="B12" s="35">
+      <c r="B12" s="47">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D12" s="3">
+      <c r="C12" s="47"/>
+      <c r="D12" s="48">
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G12" s="25">
-        <f>MATCH((A12-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+      <c r="G12" s="49">
+        <f>MATCH((A12-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>90</v>
       </c>
-      <c r="H12" t="e">
-        <f>MATCH(A12,FOMC_Meetings!$A$2:$A$197,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="3"/>
-        <v>-50</v>
+      <c r="H12" s="49" t="e">
+        <f>MATCH(A12,FOMC_Meetings!$A$2:$A$196,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I12" s="49">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J12" s="49">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="49">
+        <f>VLOOKUP(IF(I12=1,(A12-1),A12),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1040,11 +1059,11 @@
         <v>0</v>
       </c>
       <c r="G13" t="e">
-        <f>MATCH((A13-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A13-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H13" s="25">
-        <f>MATCH(A13,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A13,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>96</v>
       </c>
       <c r="I13">
@@ -1056,8 +1075,8 @@
         <v>1</v>
       </c>
       <c r="K13">
-        <f t="shared" si="3"/>
-        <v>-25</v>
+        <f>VLOOKUP(IF(I13=1,(A13-1),A13),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1075,11 +1094,11 @@
         <v>0</v>
       </c>
       <c r="G14" t="e">
-        <f>MATCH((A14-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A14-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H14" s="25">
-        <f>MATCH(A14,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A14,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>97</v>
       </c>
       <c r="I14">
@@ -1091,8 +1110,8 @@
         <v>1</v>
       </c>
       <c r="K14">
-        <f t="shared" si="3"/>
-        <v>-75</v>
+        <f>VLOOKUP(IF(I14=1,(A14-1),A14),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1110,11 +1129,11 @@
         <v>0</v>
       </c>
       <c r="G15" t="e">
-        <f>MATCH((A15-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A15-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H15" s="25">
-        <f>MATCH(A15,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A15,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>99</v>
       </c>
       <c r="I15">
@@ -1126,43 +1145,44 @@
         <v>1</v>
       </c>
       <c r="K15">
-        <f t="shared" si="3"/>
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+        <f>VLOOKUP(IF(I15=1,(A15-1),A15),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="46">
         <v>39469</v>
       </c>
-      <c r="B16" s="35">
+      <c r="B16" s="47">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="D16" s="3">
+      <c r="C16" s="47"/>
+      <c r="D16" s="48">
         <v>-7.4999999999999997E-3</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G16" s="25">
-        <f>MATCH((A16-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+      <c r="G16" s="49">
+        <f>MATCH((A16-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>100</v>
       </c>
-      <c r="H16" t="e">
-        <f>MATCH(A16,FOMC_Meetings!$A$2:$A$197,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="3"/>
-        <v>-75</v>
+      <c r="H16" s="49" t="e">
+        <f>MATCH(A16,FOMC_Meetings!$A$2:$A$196,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I16" s="49">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J16" s="49">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="49">
+        <f>VLOOKUP(IF(I16=1,(A16-1),A16),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1180,11 +1200,11 @@
         <v>0</v>
       </c>
       <c r="G17" t="e">
-        <f>MATCH((A17-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A17-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H17" s="25">
-        <f>MATCH(A17,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A17,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>102</v>
       </c>
       <c r="I17">
@@ -1196,8 +1216,8 @@
         <v>1</v>
       </c>
       <c r="K17">
-        <f t="shared" si="3"/>
-        <v>-25</v>
+        <f>VLOOKUP(IF(I17=1,(A17-1),A17),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1215,11 +1235,11 @@
         <v>0</v>
       </c>
       <c r="G18" t="e">
-        <f>MATCH((A18-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A18-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H18" s="25">
-        <f>MATCH(A18,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A18,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>104</v>
       </c>
       <c r="I18">
@@ -1231,8 +1251,8 @@
         <v>1</v>
       </c>
       <c r="K18">
-        <f t="shared" si="3"/>
-        <v>-25</v>
+        <f>VLOOKUP(IF(I18=1,(A18-1),A18),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1250,11 +1270,11 @@
         <v>0</v>
       </c>
       <c r="G19" t="e">
-        <f>MATCH((A19-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A19-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H19" s="25">
-        <f>MATCH(A19,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A19,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>105</v>
       </c>
       <c r="I19">
@@ -1266,8 +1286,8 @@
         <v>1</v>
       </c>
       <c r="K19">
-        <f t="shared" si="3"/>
-        <v>-50</v>
+        <f>VLOOKUP(IF(I19=1,(A19-1),A19),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1285,11 +1305,11 @@
         <v>0</v>
       </c>
       <c r="G20" t="e">
-        <f>MATCH((A20-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A20-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H20" s="25">
-        <f>MATCH(A20,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A20,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>117</v>
       </c>
       <c r="I20">
@@ -1301,8 +1321,8 @@
         <v>1</v>
       </c>
       <c r="K20">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I20=1,(A20-1),A20),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1320,11 +1340,11 @@
         <v>0</v>
       </c>
       <c r="G21" t="e">
-        <f>MATCH((A21-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A21-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H21" s="25">
-        <f>MATCH(A21,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A21,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>118</v>
       </c>
       <c r="I21">
@@ -1336,8 +1356,8 @@
         <v>1</v>
       </c>
       <c r="K21">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I21=1,(A21-1),A21),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1355,11 +1375,11 @@
         <v>0</v>
       </c>
       <c r="G22" t="e">
-        <f>MATCH((A22-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A22-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H22" s="25">
-        <f>MATCH(A22,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A22,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>119</v>
       </c>
       <c r="I22">
@@ -1371,8 +1391,8 @@
         <v>1</v>
       </c>
       <c r="K22">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I22=1,(A22-1),A22),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1390,11 +1410,11 @@
         <v>0</v>
       </c>
       <c r="G23" t="e">
-        <f>MATCH((A23-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A23-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H23" s="25">
-        <f>MATCH(A23,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A23,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>120</v>
       </c>
       <c r="I23">
@@ -1406,8 +1426,8 @@
         <v>1</v>
       </c>
       <c r="K23">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I23=1,(A23-1),A23),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1425,11 +1445,11 @@
         <v>0</v>
       </c>
       <c r="G24" t="e">
-        <f>MATCH((A24-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A24-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H24" s="25">
-        <f>MATCH(A24,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A24,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>121</v>
       </c>
       <c r="I24">
@@ -1441,8 +1461,8 @@
         <v>1</v>
       </c>
       <c r="K24">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I24=1,(A24-1),A24),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1460,11 +1480,11 @@
         <v>0</v>
       </c>
       <c r="G25" t="e">
-        <f>MATCH((A25-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A25-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H25" s="25">
-        <f>MATCH(A25,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A25,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>122</v>
       </c>
       <c r="I25">
@@ -1476,8 +1496,8 @@
         <v>1</v>
       </c>
       <c r="K25">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I25=1,(A25-1),A25),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1495,11 +1515,11 @@
         <v>0</v>
       </c>
       <c r="G26" t="e">
-        <f>MATCH((A26-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A26-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H26" s="25">
-        <f>MATCH(A26,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A26,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>123</v>
       </c>
       <c r="I26">
@@ -1511,8 +1531,8 @@
         <v>1</v>
       </c>
       <c r="K26">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I26=1,(A26-1),A26),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1526,15 +1546,15 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F27" s="2">
-        <f t="shared" ref="F27:F56" si="5">B28+D27-B27</f>
+        <f t="shared" ref="F27:F56" si="3">B28+D27-B27</f>
         <v>0</v>
       </c>
       <c r="G27" t="e">
-        <f>MATCH((A27-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A27-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H27" s="25">
-        <f>MATCH(A27,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A27,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>124</v>
       </c>
       <c r="I27">
@@ -1546,8 +1566,8 @@
         <v>1</v>
       </c>
       <c r="K27">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I27=1,(A27-1),A27),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1561,15 +1581,15 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F28" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G28" t="e">
-        <f>MATCH((A28-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A28-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H28" s="25">
-        <f>MATCH(A28,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A28,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>125</v>
       </c>
       <c r="I28">
@@ -1581,8 +1601,8 @@
         <v>1</v>
       </c>
       <c r="K28">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I28=1,(A28-1),A28),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -1596,15 +1616,15 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F29" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G29" t="e">
-        <f>MATCH((A29-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A29-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H29" s="25">
-        <f>MATCH(A29,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A29,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>126</v>
       </c>
       <c r="I29">
@@ -1616,8 +1636,8 @@
         <v>1</v>
       </c>
       <c r="K29">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I29=1,(A29-1),A29),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -1631,15 +1651,15 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F30" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G30" t="e">
-        <f>MATCH((A30-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A30-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H30" s="25">
-        <f>MATCH(A30,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A30,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>127</v>
       </c>
       <c r="I30">
@@ -1651,8 +1671,8 @@
         <v>1</v>
       </c>
       <c r="K30">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I30=1,(A30-1),A30),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -1667,15 +1687,15 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F31" s="42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G31" s="43" t="e">
-        <f>MATCH((A31-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A31-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H31" s="43">
-        <f>MATCH(A31,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A31,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>128</v>
       </c>
       <c r="I31" s="43">
@@ -1686,9 +1706,9 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="K31" s="43">
-        <f t="shared" si="3"/>
-        <v>25</v>
+      <c r="K31">
+        <f>VLOOKUP(IF(I31=1,(A31-1),A31),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1702,15 +1722,15 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F32" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G32" t="e">
-        <f>MATCH((A32-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A32-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H32" s="25">
-        <f>MATCH(A32,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A32,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>129</v>
       </c>
       <c r="I32">
@@ -1722,8 +1742,8 @@
         <v>1</v>
       </c>
       <c r="K32">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I32=1,(A32-1),A32),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -1737,15 +1757,15 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F33" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G33" t="e">
-        <f>MATCH((A33-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A33-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H33" s="25">
-        <f>MATCH(A33,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A33,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>130</v>
       </c>
       <c r="I33">
@@ -1757,8 +1777,8 @@
         <v>1</v>
       </c>
       <c r="K33">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I33=1,(A33-1),A33),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -1772,15 +1792,15 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F34" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G34" t="e">
-        <f>MATCH((A34-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A34-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H34" s="25">
-        <f>MATCH(A34,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A34,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>131</v>
       </c>
       <c r="I34">
@@ -1792,8 +1812,8 @@
         <v>1</v>
       </c>
       <c r="K34">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I34=1,(A34-1),A34),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -1807,15 +1827,15 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F35" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G35" t="e">
-        <f>MATCH((A35-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A35-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H35" s="25">
-        <f>MATCH(A35,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A35,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>132</v>
       </c>
       <c r="I35">
@@ -1827,8 +1847,8 @@
         <v>1</v>
       </c>
       <c r="K35">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I35=1,(A35-1),A35),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -1842,15 +1862,15 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F36" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G36" t="e">
-        <f>MATCH((A36-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A36-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H36" s="25">
-        <f>MATCH(A36,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A36,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>133</v>
       </c>
       <c r="I36">
@@ -1862,8 +1882,8 @@
         <v>1</v>
       </c>
       <c r="K36">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I36=1,(A36-1),A36),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -1882,12 +1902,12 @@
         <v>0</v>
       </c>
       <c r="G37" t="e">
-        <f>MATCH((A37-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A37-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H37" s="25">
-        <f>MATCH(A37,FOMC_Meetings!$A$2:$A$197,0)</f>
-        <v>142</v>
+        <f>MATCH(A37,FOMC_Meetings!$A$2:$A$196,0)</f>
+        <v>141</v>
       </c>
       <c r="I37">
         <f t="shared" si="1"/>
@@ -1898,8 +1918,8 @@
         <v>1</v>
       </c>
       <c r="K37">
-        <f t="shared" si="3"/>
-        <v>-25</v>
+        <f>VLOOKUP(IF(I37=1,(A37-1),A37),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -1914,16 +1934,16 @@
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F38" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G38" t="e">
-        <f>MATCH((A38-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A38-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H38" s="25">
-        <f>MATCH(A38,FOMC_Meetings!$A$2:$A$197,0)</f>
-        <v>151</v>
+        <f>MATCH(A38,FOMC_Meetings!$A$2:$A$196,0)</f>
+        <v>150</v>
       </c>
       <c r="I38">
         <f t="shared" si="1"/>
@@ -1934,8 +1954,8 @@
         <v>1</v>
       </c>
       <c r="K38">
-        <f t="shared" si="3"/>
-        <v>-50</v>
+        <f>VLOOKUP(IF(I38=1,(A38-1),A38),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -1950,16 +1970,16 @@
         <v>-2.5000000000000001E-3</v>
       </c>
       <c r="F39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G39" t="e">
-        <f>MATCH((A39-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A39-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H39" s="25">
-        <f>MATCH(A39,FOMC_Meetings!$A$2:$A$197,0)</f>
-        <v>158</v>
+        <f>MATCH(A39,FOMC_Meetings!$A$2:$A$196,0)</f>
+        <v>157</v>
       </c>
       <c r="I39">
         <f t="shared" si="1"/>
@@ -1970,8 +1990,8 @@
         <v>1</v>
       </c>
       <c r="K39">
-        <f t="shared" si="3"/>
-        <v>-25</v>
+        <f>VLOOKUP(IF(I39=1,(A39-1),A39),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -1985,16 +2005,16 @@
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F40" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G40" t="e">
-        <f>MATCH((A40-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A40-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H40" s="25">
-        <f>MATCH(A40,FOMC_Meetings!$A$2:$A$197,0)</f>
-        <v>159</v>
+        <f>MATCH(A40,FOMC_Meetings!$A$2:$A$196,0)</f>
+        <v>158</v>
       </c>
       <c r="I40">
         <f t="shared" si="1"/>
@@ -2005,8 +2025,8 @@
         <v>1</v>
       </c>
       <c r="K40">
-        <f t="shared" si="3"/>
-        <v>-50</v>
+        <f>VLOOKUP(IF(I40=1,(A40-1),A40),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -2020,63 +2040,64 @@
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F41" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G41" t="e">
-        <f>MATCH((A41-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A41-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H41" s="25">
-        <f>MATCH(A41,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A41,FOMC_Meetings!$A$2:$A$196,0)</f>
+        <v>159</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K41">
+        <f>VLOOKUP(IF(I41=1,(A41-1),A41),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="46">
+        <v>37151</v>
+      </c>
+      <c r="B42" s="47">
+        <v>0.03</v>
+      </c>
+      <c r="C42" s="47"/>
+      <c r="D42" s="48">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="F42" s="48">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G42" s="49" t="e">
+        <f>MATCH((A42-1), FOMC_Meetings!$A$2:$A$196,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H42" s="49">
+        <f>MATCH(A42,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>160</v>
       </c>
-      <c r="I41">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J41">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K41">
-        <f t="shared" si="3"/>
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
-        <v>37151</v>
-      </c>
-      <c r="B42" s="38">
-        <v>0.03</v>
-      </c>
-      <c r="D42" s="3">
-        <v>-5.0000000000000001E-3</v>
-      </c>
-      <c r="F42" s="2">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G42" t="e">
-        <f>MATCH((A42-1), FOMC_Meetings!$A$2:$A$197,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H42" s="25">
-        <f>MATCH(A42,FOMC_Meetings!$A$2:$A$197,0)</f>
-        <v>161</v>
-      </c>
-      <c r="I42">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J42">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K42">
-        <f t="shared" si="3"/>
-        <v>-50</v>
+      <c r="I42" s="49">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J42" s="49">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K42" s="49">
+        <f>VLOOKUP(IF(I42=1,(A42-1),A42),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -2090,16 +2111,16 @@
         <v>-2.5000000000000001E-3</v>
       </c>
       <c r="F43" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G43" t="e">
-        <f>MATCH((A43-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A43-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H43" s="25">
-        <f>MATCH(A43,FOMC_Meetings!$A$2:$A$197,0)</f>
-        <v>163</v>
+        <f>MATCH(A43,FOMC_Meetings!$A$2:$A$196,0)</f>
+        <v>162</v>
       </c>
       <c r="I43">
         <f t="shared" si="1"/>
@@ -2110,8 +2131,8 @@
         <v>1</v>
       </c>
       <c r="K43">
-        <f t="shared" si="3"/>
-        <v>-25</v>
+        <f>VLOOKUP(IF(I43=1,(A43-1),A43),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -2125,16 +2146,16 @@
         <v>-2.5000000000000001E-3</v>
       </c>
       <c r="F44" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G44" t="e">
-        <f>MATCH((A44-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A44-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H44" s="25">
-        <f>MATCH(A44,FOMC_Meetings!$A$2:$A$197,0)</f>
-        <v>164</v>
+        <f>MATCH(A44,FOMC_Meetings!$A$2:$A$196,0)</f>
+        <v>163</v>
       </c>
       <c r="I44">
         <f t="shared" si="1"/>
@@ -2145,8 +2166,8 @@
         <v>1</v>
       </c>
       <c r="K44">
-        <f t="shared" si="3"/>
-        <v>-25</v>
+        <f>VLOOKUP(IF(I44=1,(A44-1),A44),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -2160,63 +2181,64 @@
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F45" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G45" t="e">
-        <f>MATCH((A45-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A45-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H45" s="25">
-        <f>MATCH(A45,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A45,FOMC_Meetings!$A$2:$A$196,0)</f>
+        <v>164</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K45">
+        <f>VLOOKUP(IF(I45=1,(A45-1),A45),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="46">
+        <v>36999</v>
+      </c>
+      <c r="B46" s="47">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C46" s="47"/>
+      <c r="D46" s="48">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="F46" s="48">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G46" s="49" t="e">
+        <f>MATCH((A46-1), FOMC_Meetings!$A$2:$A$196,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H46" s="49">
+        <f>MATCH(A46,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>165</v>
       </c>
-      <c r="I45">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J45">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K45">
-        <f t="shared" si="3"/>
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
-        <v>36999</v>
-      </c>
-      <c r="B46" s="38">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="D46" s="3">
-        <v>-5.0000000000000001E-3</v>
-      </c>
-      <c r="F46" s="2">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G46" t="e">
-        <f>MATCH((A46-1), FOMC_Meetings!$A$2:$A$197,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H46" s="25">
-        <f>MATCH(A46,FOMC_Meetings!$A$2:$A$197,0)</f>
-        <v>166</v>
-      </c>
-      <c r="I46">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J46">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K46">
-        <f t="shared" si="3"/>
-        <v>-50</v>
+      <c r="I46" s="49">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J46" s="49">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K46" s="49">
+        <f>VLOOKUP(IF(I46=1,(A46-1),A46),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -2230,16 +2252,16 @@
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F47" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G47" t="e">
-        <f>MATCH((A47-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A47-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H47" s="25">
-        <f>MATCH(A47,FOMC_Meetings!$A$2:$A$197,0)</f>
-        <v>168</v>
+        <f>MATCH(A47,FOMC_Meetings!$A$2:$A$196,0)</f>
+        <v>167</v>
       </c>
       <c r="I47">
         <f t="shared" si="1"/>
@@ -2250,8 +2272,8 @@
         <v>1</v>
       </c>
       <c r="K47">
-        <f t="shared" si="3"/>
-        <v>-50</v>
+        <f>VLOOKUP(IF(I47=1,(A47-1),A47),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -2265,64 +2287,64 @@
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F48" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G48" t="e">
-        <f>MATCH((A48-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A48-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H48" s="25">
-        <f>MATCH(A48,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A48,FOMC_Meetings!$A$2:$A$196,0)</f>
+        <v>168</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <f>VLOOKUP(IF(I48=1,(A48-1),A48),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="46">
+        <v>36894</v>
+      </c>
+      <c r="B49" s="47">
+        <v>0.06</v>
+      </c>
+      <c r="C49" s="47"/>
+      <c r="D49" s="48">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="F49" s="48">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G49" s="49" t="e">
+        <f>MATCH((A49-1), FOMC_Meetings!$A$2:$A$196,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H49" s="49">
+        <f>MATCH(A49,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>169</v>
       </c>
-      <c r="I48">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J48">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K48">
-        <f t="shared" si="3"/>
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="12">
-        <v>36894</v>
-      </c>
-      <c r="B49" s="39">
-        <v>0.06</v>
-      </c>
-      <c r="C49" s="39"/>
-      <c r="D49" s="13">
-        <v>-5.0000000000000001E-3</v>
-      </c>
-      <c r="F49" s="2">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G49" t="e">
-        <f>MATCH((A49-1), FOMC_Meetings!$A$2:$A$197,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H49" s="25">
-        <f>MATCH(A49,FOMC_Meetings!$A$2:$A$197,0)</f>
-        <v>170</v>
-      </c>
-      <c r="I49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J49">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K49">
-        <f t="shared" si="3"/>
-        <v>-50</v>
+      <c r="I49" s="49">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J49" s="49">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K49" s="49">
+        <f>VLOOKUP(IF(I49=1,(A49-1),A49),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -2337,16 +2359,16 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F50" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G50" t="e">
-        <f>MATCH((A50-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A50-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H50" s="25">
-        <f>MATCH(A50,FOMC_Meetings!$A$2:$A$197,0)</f>
-        <v>176</v>
+        <f>MATCH(A50,FOMC_Meetings!$A$2:$A$196,0)</f>
+        <v>175</v>
       </c>
       <c r="I50">
         <f t="shared" si="1"/>
@@ -2357,8 +2379,8 @@
         <v>1</v>
       </c>
       <c r="K50">
-        <f t="shared" si="3"/>
-        <v>50</v>
+        <f>VLOOKUP(IF(I50=1,(A50-1),A50),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -2372,16 +2394,16 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F51" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G51" t="e">
-        <f>MATCH((A51-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A51-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H51" s="25">
-        <f>MATCH(A51,FOMC_Meetings!$A$2:$A$197,0)</f>
-        <v>177</v>
+        <f>MATCH(A51,FOMC_Meetings!$A$2:$A$196,0)</f>
+        <v>176</v>
       </c>
       <c r="I51">
         <f t="shared" si="1"/>
@@ -2392,8 +2414,8 @@
         <v>1</v>
       </c>
       <c r="K51">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I51=1,(A51-1),A51),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -2407,16 +2429,16 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F52" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G52" t="e">
-        <f>MATCH((A52-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A52-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H52" s="25">
-        <f>MATCH(A52,FOMC_Meetings!$A$2:$A$197,0)</f>
-        <v>178</v>
+        <f>MATCH(A52,FOMC_Meetings!$A$2:$A$196,0)</f>
+        <v>177</v>
       </c>
       <c r="I52">
         <f t="shared" si="1"/>
@@ -2427,8 +2449,8 @@
         <v>1</v>
       </c>
       <c r="K52">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I52=1,(A52-1),A52),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -2442,16 +2464,16 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F53" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G53" t="e">
-        <f>MATCH((A53-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A53-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H53" s="25">
-        <f>MATCH(A53,FOMC_Meetings!$A$2:$A$197,0)</f>
-        <v>180</v>
+        <f>MATCH(A53,FOMC_Meetings!$A$2:$A$196,0)</f>
+        <v>179</v>
       </c>
       <c r="I53">
         <f t="shared" si="1"/>
@@ -2462,8 +2484,8 @@
         <v>1</v>
       </c>
       <c r="K53">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I53=1,(A53-1),A53),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -2477,16 +2499,16 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F54" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G54" t="e">
-        <f>MATCH((A54-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A54-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H54" s="25">
-        <f>MATCH(A54,FOMC_Meetings!$A$2:$A$197,0)</f>
-        <v>182</v>
+        <f>MATCH(A54,FOMC_Meetings!$A$2:$A$196,0)</f>
+        <v>181</v>
       </c>
       <c r="I54">
         <f t="shared" si="1"/>
@@ -2497,8 +2519,8 @@
         <v>1</v>
       </c>
       <c r="K54">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I54=1,(A54-1),A54),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -2512,16 +2534,16 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F55" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G55" t="e">
-        <f>MATCH((A55-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A55-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H55" s="25">
-        <f>MATCH(A55,FOMC_Meetings!$A$2:$A$197,0)</f>
-        <v>183</v>
+        <f>MATCH(A55,FOMC_Meetings!$A$2:$A$196,0)</f>
+        <v>182</v>
       </c>
       <c r="I55">
         <f t="shared" si="1"/>
@@ -2532,8 +2554,8 @@
         <v>1</v>
       </c>
       <c r="K55">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>VLOOKUP(IF(I55=1,(A55-1),A55),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -2547,63 +2569,64 @@
         <v>-2.5000000000000001E-3</v>
       </c>
       <c r="F56" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G56" t="e">
-        <f>MATCH((A56-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A56-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H56" s="25">
-        <f>MATCH(A56,FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH(A56,FOMC_Meetings!$A$2:$A$196,0)</f>
+        <v>187</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K56">
+        <f>VLOOKUP(IF(I56=1,(A56-1),A56),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="46">
+        <v>36083</v>
+      </c>
+      <c r="B57" s="47">
+        <v>0.05</v>
+      </c>
+      <c r="C57" s="47"/>
+      <c r="D57" s="48">
+        <v>-2.5000000000000001E-3</v>
+      </c>
+      <c r="F57" s="48">
+        <f>B58+D57-B57</f>
+        <v>0</v>
+      </c>
+      <c r="G57" s="49" t="e">
+        <f>MATCH((A57-1), FOMC_Meetings!$A$2:$A$196,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H57" s="49">
+        <f>MATCH(A57,FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>188</v>
       </c>
-      <c r="I56">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J56">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K56">
-        <f t="shared" si="3"/>
-        <v>-25</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
-        <v>36083</v>
-      </c>
-      <c r="B57" s="35">
-        <v>0.05</v>
-      </c>
-      <c r="D57" s="7">
-        <v>-2.5000000000000001E-3</v>
-      </c>
-      <c r="F57" s="2">
-        <f>B58+D57-B57</f>
-        <v>0</v>
-      </c>
-      <c r="G57" t="e">
-        <f>MATCH((A57-1), FOMC_Meetings!$A$2:$A$197,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H57" s="25">
-        <f>MATCH(A57,FOMC_Meetings!$A$2:$A$197,0)</f>
-        <v>189</v>
-      </c>
-      <c r="I57">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J57">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K57">
-        <f t="shared" si="3"/>
-        <v>-25</v>
+      <c r="I57" s="49">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J57" s="49">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K57" s="49">
+        <f>VLOOKUP(IF(I57=1,(A57-1),A57),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -2617,12 +2640,12 @@
         <v>-2.5000000000000001E-3</v>
       </c>
       <c r="G58" t="e">
-        <f>MATCH((A58-1), FOMC_Meetings!$A$2:$A$197,0)</f>
+        <f>MATCH((A58-1), FOMC_Meetings!$A$2:$A$196,0)</f>
         <v>#N/A</v>
       </c>
       <c r="H58" s="25">
-        <f>MATCH(A58,FOMC_Meetings!$A$2:$A$197,0)</f>
-        <v>190</v>
+        <f>MATCH(A58,FOMC_Meetings!$A$2:$A$196,0)</f>
+        <v>189</v>
       </c>
       <c r="I58">
         <f t="shared" si="1"/>
@@ -2633,8 +2656,8 @@
         <v>1</v>
       </c>
       <c r="K58">
-        <f t="shared" si="3"/>
-        <v>-25</v>
+        <f>VLOOKUP(IF(I58=1,(A58-1),A58),FOMC_Meetings!$A$2:$B$196,2,FALSE)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -2648,1303 +2671,1901 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96504E55-3F76-42FC-885A-83EA18AD498E}">
-  <dimension ref="A1:D197"/>
+  <dimension ref="A1:E196"/>
   <sheetViews>
-    <sheetView topLeftCell="A161" workbookViewId="0">
-      <selection activeCell="A170" sqref="A170:A197"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A141" sqref="A141:XFD141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>43369</v>
       </c>
-      <c r="B2" s="17">
-        <v>1</v>
-      </c>
-      <c r="D2" s="17" t="s">
+      <c r="B2" s="44">
+        <v>0</v>
+      </c>
+      <c r="C2" s="17">
+        <v>1</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>43313</v>
       </c>
-      <c r="B3" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="44">
+        <v>0</v>
+      </c>
+      <c r="C3" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>43264</v>
       </c>
-      <c r="B4" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="44">
+        <v>0</v>
+      </c>
+      <c r="C4" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>43222</v>
       </c>
-      <c r="B5" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="44">
+        <v>0</v>
+      </c>
+      <c r="C5" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>43180</v>
       </c>
-      <c r="B6" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="44">
+        <v>0</v>
+      </c>
+      <c r="C6" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>43131</v>
       </c>
-      <c r="B7" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="44">
+        <v>0</v>
+      </c>
+      <c r="C7" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18">
         <v>43082</v>
       </c>
-      <c r="B8" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="44">
+        <v>0</v>
+      </c>
+      <c r="C8" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18">
         <v>43040</v>
       </c>
-      <c r="B9" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="44">
+        <v>0</v>
+      </c>
+      <c r="C9" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18">
         <v>42998</v>
       </c>
-      <c r="B10" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="44">
+        <v>0</v>
+      </c>
+      <c r="C10" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
         <v>42942</v>
       </c>
-      <c r="B11" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="44">
+        <v>0</v>
+      </c>
+      <c r="C11" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
         <v>42900</v>
       </c>
-      <c r="B12" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="44">
+        <v>0</v>
+      </c>
+      <c r="C12" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18">
         <v>42858</v>
       </c>
-      <c r="B13" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="44">
+        <v>0</v>
+      </c>
+      <c r="C13" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18">
         <v>42809</v>
       </c>
-      <c r="B14" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="44">
+        <v>0</v>
+      </c>
+      <c r="C14" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="18">
         <v>42767</v>
       </c>
-      <c r="B15" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="44">
+        <v>0</v>
+      </c>
+      <c r="C15" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <v>42718</v>
       </c>
-      <c r="B16" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="44">
+        <v>0</v>
+      </c>
+      <c r="C16" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
         <v>42676</v>
       </c>
-      <c r="B17" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="44">
+        <v>0</v>
+      </c>
+      <c r="C17" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
-        <v>42999</v>
-      </c>
-      <c r="B18" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+        <v>42634</v>
+      </c>
+      <c r="B18" s="44">
+        <v>0</v>
+      </c>
+      <c r="C18" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
         <v>42578</v>
       </c>
-      <c r="B19" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="44">
+        <v>0</v>
+      </c>
+      <c r="C19" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
         <v>42536</v>
       </c>
-      <c r="B20" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="44">
+        <v>0</v>
+      </c>
+      <c r="C20" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16">
         <v>42487</v>
       </c>
-      <c r="B21" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="44">
+        <v>0</v>
+      </c>
+      <c r="C21" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <v>42445</v>
       </c>
-      <c r="B22" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="44">
+        <v>0</v>
+      </c>
+      <c r="C22" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16">
         <v>42396</v>
       </c>
-      <c r="B23" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="44">
+        <v>0</v>
+      </c>
+      <c r="C23" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18">
         <v>42354</v>
       </c>
-      <c r="B24" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="44">
+        <v>0</v>
+      </c>
+      <c r="C24" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18">
         <v>42305</v>
       </c>
-      <c r="B25" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="44">
+        <v>0</v>
+      </c>
+      <c r="C25" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18">
         <v>42264</v>
       </c>
-      <c r="B26" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="44">
+        <v>0</v>
+      </c>
+      <c r="C26" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18">
         <v>42214</v>
       </c>
-      <c r="B27" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="44">
+        <v>0</v>
+      </c>
+      <c r="C27" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18">
         <v>42172</v>
       </c>
-      <c r="B28" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="44">
+        <v>0</v>
+      </c>
+      <c r="C28" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="28">
         <v>42123</v>
       </c>
-      <c r="B29" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="44">
+        <v>0</v>
+      </c>
+      <c r="C29" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18">
         <v>42081</v>
       </c>
-      <c r="B30" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="44">
+        <v>0</v>
+      </c>
+      <c r="C30" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18">
         <v>42032</v>
       </c>
-      <c r="B31" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="44">
+        <v>0</v>
+      </c>
+      <c r="C31" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
         <v>41990</v>
       </c>
-      <c r="B32" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="44">
+        <v>0</v>
+      </c>
+      <c r="C32" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16">
         <v>41941</v>
       </c>
-      <c r="B33" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="44">
+        <v>0</v>
+      </c>
+      <c r="C33" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <v>41899</v>
       </c>
-      <c r="B34" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="44">
+        <v>0</v>
+      </c>
+      <c r="C34" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16">
         <v>41850</v>
       </c>
-      <c r="B35" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="44">
+        <v>0</v>
+      </c>
+      <c r="C35" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16">
         <v>41808</v>
       </c>
-      <c r="B36" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="44">
+        <v>0</v>
+      </c>
+      <c r="C36" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
         <v>41759</v>
       </c>
-      <c r="B37" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="44">
+        <v>0</v>
+      </c>
+      <c r="C37" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="16">
         <v>41717</v>
       </c>
-      <c r="B38" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="44">
+        <v>0</v>
+      </c>
+      <c r="C38" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="21">
         <v>41702</v>
       </c>
-      <c r="B39" s="22">
-        <v>0</v>
-      </c>
-      <c r="C39" s="22" t="s">
+      <c r="B39" s="44">
+        <v>1</v>
+      </c>
+      <c r="C39" s="22">
+        <v>0</v>
+      </c>
+      <c r="D39" s="22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="16">
         <v>41668</v>
       </c>
-      <c r="B40" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="44">
+        <v>0</v>
+      </c>
+      <c r="C40" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="18">
         <v>41626</v>
       </c>
-      <c r="B41" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="44">
+        <v>0</v>
+      </c>
+      <c r="C41" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="18">
         <v>41577</v>
       </c>
-      <c r="B42" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="44">
+        <v>0</v>
+      </c>
+      <c r="C42" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="23">
         <v>41563</v>
       </c>
-      <c r="B43" s="20">
-        <v>0</v>
-      </c>
-      <c r="C43" s="20" t="s">
+      <c r="B43" s="44">
+        <v>1</v>
+      </c>
+      <c r="C43" s="20">
+        <v>0</v>
+      </c>
+      <c r="D43" s="20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="18">
         <v>41535</v>
       </c>
-      <c r="B44" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="44">
+        <v>0</v>
+      </c>
+      <c r="C44" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="18">
         <v>41486</v>
       </c>
-      <c r="B45" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="44">
+        <v>0</v>
+      </c>
+      <c r="C45" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="18">
         <v>41444</v>
       </c>
-      <c r="B46" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="44">
+        <v>0</v>
+      </c>
+      <c r="C46" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="18">
         <v>41395</v>
       </c>
-      <c r="B47" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="44">
+        <v>0</v>
+      </c>
+      <c r="C47" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="18">
         <v>41353</v>
       </c>
-      <c r="B48" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="44">
+        <v>0</v>
+      </c>
+      <c r="C48" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="18">
         <v>41304</v>
       </c>
-      <c r="B49" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="44">
+        <v>0</v>
+      </c>
+      <c r="C49" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="16">
         <v>41255</v>
       </c>
-      <c r="B50" s="17">
-        <v>1</v>
-      </c>
-      <c r="D50" s="17" t="s">
+      <c r="B50" s="44">
+        <v>0</v>
+      </c>
+      <c r="C50" s="17">
+        <v>1</v>
+      </c>
+      <c r="E50" s="17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
         <v>41206</v>
       </c>
-      <c r="B51" s="17">
-        <v>0</v>
-      </c>
-      <c r="D51" s="17" t="s">
+      <c r="B51" s="44">
+        <v>0</v>
+      </c>
+      <c r="C51" s="17">
+        <v>0</v>
+      </c>
+      <c r="E51" s="17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
         <v>41165</v>
       </c>
-      <c r="B52" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="44">
+        <v>0</v>
+      </c>
+      <c r="C52" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
         <v>41122</v>
       </c>
-      <c r="B53" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="44">
+        <v>0</v>
+      </c>
+      <c r="C53" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="16">
         <v>41080</v>
       </c>
-      <c r="B54" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="44">
+        <v>0</v>
+      </c>
+      <c r="C54" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="16">
         <v>41024</v>
       </c>
-      <c r="B55" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="44">
+        <v>0</v>
+      </c>
+      <c r="C55" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="16">
         <v>40981</v>
       </c>
-      <c r="B56" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="44">
+        <v>0</v>
+      </c>
+      <c r="C56" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="28">
         <v>40933</v>
       </c>
-      <c r="B57" s="29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="44">
+        <v>0</v>
+      </c>
+      <c r="C57" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="18">
         <v>40890</v>
       </c>
-      <c r="B58" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="44">
+        <v>0</v>
+      </c>
+      <c r="C58" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="23">
         <v>40875</v>
       </c>
-      <c r="B59" s="20">
-        <v>0</v>
-      </c>
-      <c r="C59" s="20" t="s">
+      <c r="B59" s="44">
+        <v>1</v>
+      </c>
+      <c r="C59" s="20">
+        <v>0</v>
+      </c>
+      <c r="D59" s="20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="18">
         <v>40849</v>
       </c>
-      <c r="B60" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="44">
+        <v>0</v>
+      </c>
+      <c r="C60" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="18">
         <v>40807</v>
       </c>
-      <c r="B61" s="19">
-        <v>0</v>
-      </c>
-      <c r="C61" s="19"/>
-    </row>
-    <row r="62" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="44">
+        <v>0</v>
+      </c>
+      <c r="C61" s="19">
+        <v>0</v>
+      </c>
+      <c r="D61" s="19"/>
+    </row>
+    <row r="62" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="18">
         <v>40764</v>
       </c>
-      <c r="B62" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="44">
+        <v>0</v>
+      </c>
+      <c r="C62" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="23">
         <v>40756</v>
       </c>
-      <c r="B63" s="20">
-        <v>0</v>
-      </c>
-      <c r="C63" s="20" t="s">
+      <c r="B63" s="44">
+        <v>1</v>
+      </c>
+      <c r="C63" s="20">
+        <v>0</v>
+      </c>
+      <c r="D63" s="20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="18">
         <v>40716</v>
       </c>
-      <c r="B64" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="44">
+        <v>0</v>
+      </c>
+      <c r="C64" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="18">
         <v>40660</v>
       </c>
-      <c r="B65" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="44">
+        <v>0</v>
+      </c>
+      <c r="C65" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="18">
-        <v>36965</v>
-      </c>
-      <c r="B66" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+        <v>40617</v>
+      </c>
+      <c r="B66" s="44">
+        <v>0</v>
+      </c>
+      <c r="C66" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="18">
         <v>40569</v>
       </c>
-      <c r="B67" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="44">
+        <v>0</v>
+      </c>
+      <c r="C67" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="16">
         <v>40526</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="16">
         <v>40485</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="21">
         <v>40466</v>
       </c>
-      <c r="C70" s="22" t="s">
+      <c r="B70" s="44">
+        <v>1</v>
+      </c>
+      <c r="D70" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="16">
         <v>40442</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="16">
         <v>40400</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="16">
         <v>40352</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="21">
         <v>40307</v>
       </c>
-      <c r="C74" s="22" t="s">
+      <c r="B74" s="44">
+        <v>1</v>
+      </c>
+      <c r="D74" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="16">
         <v>40296</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="16">
         <v>40253</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="16">
         <v>40205</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="18">
         <v>40163</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="18">
         <v>40121</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="18">
         <v>40079</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="18">
         <v>40037</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="18">
         <v>39988</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="23">
         <v>39967</v>
       </c>
-      <c r="C83" s="20" t="s">
+      <c r="B83" s="44">
+        <v>1</v>
+      </c>
+      <c r="D83" s="20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="18">
         <v>39932</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="28">
         <v>39890</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="18">
+      <c r="B85" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="23">
         <v>39851</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="44">
+        <v>1</v>
+      </c>
+      <c r="D86" s="20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="18">
         <v>39841</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="23">
         <v>39829</v>
       </c>
-      <c r="C88" s="20" t="s">
+      <c r="B88" s="44">
+        <v>1</v>
+      </c>
+      <c r="D88" s="20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="26">
         <v>39798</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="26">
         <v>39750</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="21">
         <v>39728</v>
       </c>
-      <c r="C91" s="22" t="s">
+      <c r="B91" s="44">
+        <v>1</v>
+      </c>
+      <c r="D91" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="21">
         <v>39720</v>
       </c>
-      <c r="C92" s="22" t="s">
+      <c r="B92" s="44">
+        <v>1</v>
+      </c>
+      <c r="D92" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="16">
         <v>39707</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B93" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="16">
         <v>39665</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="16">
+      <c r="B94" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="21">
         <v>39653</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="44">
+        <v>1</v>
+      </c>
+      <c r="D95" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="16">
         <v>39624</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B96" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="26">
         <v>39568</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B97" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="26">
         <v>39525</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="16">
+      <c r="B98" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="21">
         <v>39517</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="44">
+        <v>1</v>
+      </c>
+      <c r="D99" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="26">
         <v>39477</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="16">
+      <c r="B100" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="21">
         <v>39468</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="44">
+        <v>1</v>
+      </c>
+      <c r="D101" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="21">
         <v>39456</v>
       </c>
-      <c r="C102" s="22" t="s">
+      <c r="B102" s="44">
+        <v>1</v>
+      </c>
+      <c r="D102" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:3" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="30">
         <v>39427</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B103" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="23">
         <v>39422</v>
       </c>
-      <c r="C104" s="20" t="s">
+      <c r="B104" s="44">
+        <v>1</v>
+      </c>
+      <c r="D104" s="20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:3" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="30">
         <v>39386</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B105" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="30">
         <v>39343</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B106" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="27">
         <v>39310</v>
       </c>
-      <c r="B107" s="10"/>
-      <c r="C107" s="10" t="s">
+      <c r="B107" s="44">
+        <v>1</v>
+      </c>
+      <c r="C107" s="10"/>
+      <c r="D107" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="27">
         <v>39304</v>
       </c>
-      <c r="B108" s="10"/>
-      <c r="C108" s="10" t="s">
+      <c r="B108" s="44">
+        <v>1</v>
+      </c>
+      <c r="C108" s="10"/>
+      <c r="D108" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="109" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="28">
         <v>39301</v>
       </c>
-      <c r="B109" s="29"/>
+      <c r="B109" s="44">
+        <v>0</v>
+      </c>
       <c r="C109" s="29"/>
-    </row>
-    <row r="110" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D109" s="29"/>
+    </row>
+    <row r="110" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="18">
         <v>39261</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B110" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="18">
         <v>39211</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B111" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="18">
         <v>39162</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B112" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="28">
         <v>39113</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B113" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="16">
         <v>39063</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B114" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="16">
         <v>39015</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B115" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="16">
         <v>38980</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B116" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="16">
         <v>38937</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B117" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="16">
         <v>38897</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B118" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="16">
         <v>38847</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B119" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="16">
         <v>38804</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B120" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="16">
         <v>38748</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B121" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="18">
         <v>38699</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B122" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="18">
         <v>38657</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B123" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="18">
         <v>38615</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B124" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="18">
         <v>38573</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B125" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="18">
         <v>38533</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B126" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="18">
         <v>38475</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B127" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="18">
         <v>38433</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B128" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="18">
         <v>38385</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B129" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="16">
         <v>38335</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B130" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="16">
         <v>38301</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B131" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="16">
         <v>38251</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B132" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="16">
         <v>38209</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B133" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="16">
         <v>38168</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B134" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="16">
         <v>38111</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B135" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="16">
         <v>38062</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B136" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="16">
         <v>38014</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B137" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="18">
         <v>37964</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B138" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="18">
         <v>37922</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B139" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="18">
         <v>37880</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B140" s="44">
+        <v>0</v>
+      </c>
+      <c r="D140" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="28">
-        <v>37879</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+        <v>37845</v>
+      </c>
+      <c r="B141" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="18">
-        <v>37845</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
+        <v>37797</v>
+      </c>
+      <c r="B142" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="18">
-        <v>37797</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="18">
         <v>37747</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B143" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="23">
+        <v>37727</v>
+      </c>
+      <c r="B144" s="44">
+        <v>1</v>
+      </c>
+      <c r="D144" s="20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="23">
-        <v>37727</v>
-      </c>
-      <c r="C145" s="20" t="s">
+        <v>37719</v>
+      </c>
+      <c r="B145" s="44">
+        <v>1</v>
+      </c>
+      <c r="D145" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="146" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="23">
-        <v>37719</v>
-      </c>
-      <c r="C146" s="20" t="s">
+        <v>37712</v>
+      </c>
+      <c r="B146" s="44">
+        <v>1</v>
+      </c>
+      <c r="D146" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="147" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="23">
-        <v>37712</v>
-      </c>
-      <c r="C147" s="20" t="s">
+        <v>37705</v>
+      </c>
+      <c r="B147" s="44">
+        <v>1</v>
+      </c>
+      <c r="D147" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="148" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="23">
-        <v>37705</v>
-      </c>
-      <c r="C148" s="20" t="s">
+    <row r="148" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="18">
+        <v>37698</v>
+      </c>
+      <c r="B148" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="18">
+        <v>37650</v>
+      </c>
+      <c r="B149" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="16">
+        <v>37600</v>
+      </c>
+      <c r="B150" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="16">
+        <v>37566</v>
+      </c>
+      <c r="B151" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="16">
+        <v>37523</v>
+      </c>
+      <c r="B152" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="16">
+        <v>37481</v>
+      </c>
+      <c r="B153" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="16">
+        <v>37433</v>
+      </c>
+      <c r="B154" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="16">
+        <v>37383</v>
+      </c>
+      <c r="B155" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="16">
+        <v>37334</v>
+      </c>
+      <c r="B156" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="16">
+        <v>37286</v>
+      </c>
+      <c r="B157" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="18">
+        <v>37236</v>
+      </c>
+      <c r="B158" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="18">
+        <v>37201</v>
+      </c>
+      <c r="B159" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="18">
+        <v>37166</v>
+      </c>
+      <c r="B160" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="32">
+        <v>37151</v>
+      </c>
+      <c r="B161" s="44">
+        <v>1</v>
+      </c>
+      <c r="C161" s="33"/>
+      <c r="D161" s="33" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="149" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="18">
-        <v>37698</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="18">
-        <v>37650</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="16">
-        <v>37600</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="16">
-        <v>37566</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="16">
-        <v>37523</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="16">
-        <v>37481</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="16">
-        <v>37433</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="16">
-        <v>37383</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="16">
-        <v>37334</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="16">
-        <v>37286</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="18">
-        <v>37236</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="18">
-        <v>37201</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="18">
-        <v>37166</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="32">
-        <v>37151</v>
-      </c>
-      <c r="B162" s="33"/>
-      <c r="C162" s="33" t="s">
+        <v>37147</v>
+      </c>
+      <c r="B162" s="44">
+        <v>1</v>
+      </c>
+      <c r="C162" s="33"/>
+      <c r="D162" s="33" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="163" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="32">
-        <v>37147</v>
-      </c>
-      <c r="B163" s="33"/>
-      <c r="C163" s="33" t="s">
+    <row r="163" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="18">
+        <v>37124</v>
+      </c>
+      <c r="B163" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="18">
+        <v>37069</v>
+      </c>
+      <c r="B164" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="18">
+        <v>37026</v>
+      </c>
+      <c r="B165" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="23">
+        <v>36999</v>
+      </c>
+      <c r="B166" s="44">
+        <v>1</v>
+      </c>
+      <c r="C166" s="20"/>
+      <c r="D166" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="164" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="18">
-        <v>37124</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="18">
-        <v>37069</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="18">
-        <v>37026</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="23">
-        <v>36999</v>
-      </c>
-      <c r="B167" s="20"/>
-      <c r="C167" s="20" t="s">
+        <v>36992</v>
+      </c>
+      <c r="B167" s="44">
+        <v>1</v>
+      </c>
+      <c r="C167" s="20"/>
+      <c r="D167" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="168" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="23">
-        <v>36992</v>
-      </c>
-      <c r="B168" s="20"/>
-      <c r="C168" s="20" t="s">
+    <row r="168" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="28">
+        <v>36970</v>
+      </c>
+      <c r="B168" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="18">
+        <v>36922</v>
+      </c>
+      <c r="B169" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="23">
+        <v>36894</v>
+      </c>
+      <c r="B170" s="44">
+        <v>1</v>
+      </c>
+      <c r="C170" s="20"/>
+      <c r="D170" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="169" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="28">
-        <v>36970</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="18">
-        <v>36922</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="23">
-        <v>36894</v>
-      </c>
-      <c r="B171" s="20"/>
-      <c r="C171" s="20" t="s">
+    <row r="171" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="16">
+        <v>36879</v>
+      </c>
+      <c r="B171" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="16">
+        <v>36845</v>
+      </c>
+      <c r="B172" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="16">
+        <v>36802</v>
+      </c>
+      <c r="B173" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="16">
+        <v>36760</v>
+      </c>
+      <c r="B174" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="16">
+        <v>36705</v>
+      </c>
+      <c r="B175" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="16">
+        <v>36662</v>
+      </c>
+      <c r="B176" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="16">
+        <v>36606</v>
+      </c>
+      <c r="B177" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="16">
+        <v>36558</v>
+      </c>
+      <c r="B178" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="18">
+        <v>36515</v>
+      </c>
+      <c r="B179" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A180" s="18">
+        <v>36480</v>
+      </c>
+      <c r="B180" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="18">
+        <v>36438</v>
+      </c>
+      <c r="B181" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="18">
+        <v>36396</v>
+      </c>
+      <c r="B182" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="18">
+        <v>36341</v>
+      </c>
+      <c r="B183" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="18">
+        <v>36298</v>
+      </c>
+      <c r="B184" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="18">
+        <v>36249</v>
+      </c>
+      <c r="B185" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="18">
+        <v>36194</v>
+      </c>
+      <c r="B186" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="16">
+        <v>36151</v>
+      </c>
+      <c r="B187" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="16">
+        <v>36116</v>
+      </c>
+      <c r="B188" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A189" s="21">
+        <v>36083</v>
+      </c>
+      <c r="B189" s="44">
+        <v>1</v>
+      </c>
+      <c r="D189" s="22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="172" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="16">
-        <v>36879</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="16">
-        <v>36845</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="16">
-        <v>36802</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="16">
-        <v>36760</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="16">
-        <v>36705</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="16">
-        <v>36662</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="16">
-        <v>36606</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="16">
-        <v>36558</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="18">
-        <v>36515</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="18">
-        <v>36480</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="18">
-        <v>36438</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="18">
-        <v>36396</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="18">
-        <v>36341</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="18">
-        <v>36298</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="18">
-        <v>36249</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="18">
-        <v>36194</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="16">
-        <v>36151</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="16">
-        <v>36116</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="21">
-        <v>36083</v>
-      </c>
-      <c r="C190" s="22" t="s">
+    <row r="190" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="16">
+        <v>36067</v>
+      </c>
+      <c r="B190" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="21">
+        <v>36059</v>
+      </c>
+      <c r="B191" s="44">
+        <v>1</v>
+      </c>
+      <c r="C191" s="22"/>
+      <c r="D191" s="22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="191" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="16">
-        <v>36067</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="21">
-        <v>36059</v>
-      </c>
-      <c r="B192" s="22"/>
-      <c r="C192" s="22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="193" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="16">
+        <v>36025</v>
+      </c>
+      <c r="B192" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A193" s="16">
-        <v>36025</v>
-      </c>
-    </row>
-    <row r="194" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+        <v>35977</v>
+      </c>
+      <c r="B193" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A194" s="16">
-        <v>35977</v>
-      </c>
-    </row>
-    <row r="195" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+        <v>35934</v>
+      </c>
+      <c r="B194" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A195" s="16">
-        <v>35934</v>
-      </c>
-    </row>
-    <row r="196" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
+        <v>35885</v>
+      </c>
+      <c r="B195" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A196" s="16">
-        <v>35885</v>
-      </c>
-    </row>
-    <row r="197" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="16">
         <v>35830</v>
+      </c>
+      <c r="B196" s="44">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>